<commit_message>
harmonize tests with OF 1508:22
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.22.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.22.balsamic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A381BC05-AED5-2546-BED6-3B8B743B02E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F87011C-5CCE-F64D-925D-5D807147AD9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12820" yWindow="4460" windowWidth="25420" windowHeight="15940" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8080" yWindow="4460" windowWidth="32000" windowHeight="15940" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="641">
   <si>
     <t>Document name</t>
   </si>
@@ -2536,30 +2536,6 @@
     <t>s38</t>
   </si>
   <si>
-    <t>s39</t>
-  </si>
-  <si>
-    <t>s40</t>
-  </si>
-  <si>
-    <t>s41</t>
-  </si>
-  <si>
-    <t>s42</t>
-  </si>
-  <si>
-    <t>s43</t>
-  </si>
-  <si>
-    <t>s44</t>
-  </si>
-  <si>
-    <t>s45</t>
-  </si>
-  <si>
-    <t>s46</t>
-  </si>
-  <si>
     <t>c2</t>
   </si>
   <si>
@@ -2663,33 +2639,6 @@
   </si>
   <si>
     <t>c36</t>
-  </si>
-  <si>
-    <t>c37</t>
-  </si>
-  <si>
-    <t>c38</t>
-  </si>
-  <si>
-    <t>c39</t>
-  </si>
-  <si>
-    <t>c40</t>
-  </si>
-  <si>
-    <t>c41</t>
-  </si>
-  <si>
-    <t>c42</t>
-  </si>
-  <si>
-    <t>c43</t>
-  </si>
-  <si>
-    <t>c44</t>
-  </si>
-  <si>
-    <t>c45</t>
   </si>
   <si>
     <t>plate1</t>
@@ -3377,7 +3326,7 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
@@ -3804,6 +3753,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3839,28 +3816,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="24">
@@ -4778,8 +4733,8 @@
   </sheetPr>
   <dimension ref="A1:AMM395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="S2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="AF15" sqref="AF15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1"/>
@@ -11068,38 +11023,38 @@
       <c r="AJ8" s="39"/>
     </row>
     <row r="9" spans="1:1026" s="45" customFormat="1" ht="22" customHeight="1" outlineLevel="1">
-      <c r="A9" s="169" t="s">
+      <c r="A9" s="178" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="170"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="170"/>
-      <c r="H9" s="170"/>
-      <c r="I9" s="170"/>
-      <c r="J9" s="170"/>
-      <c r="K9" s="170"/>
-      <c r="L9" s="170"/>
-      <c r="M9" s="171"/>
+      <c r="B9" s="179"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="179"/>
+      <c r="H9" s="179"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="179"/>
+      <c r="K9" s="179"/>
+      <c r="L9" s="179"/>
+      <c r="M9" s="180"/>
       <c r="N9" s="41"/>
-      <c r="O9" s="173" t="s">
+      <c r="O9" s="182" t="s">
         <v>22</v>
       </c>
-      <c r="P9" s="173"/>
+      <c r="P9" s="182"/>
       <c r="Q9" s="133"/>
-      <c r="R9" s="175" t="s">
+      <c r="R9" s="184" t="s">
         <v>23</v>
       </c>
-      <c r="S9" s="176"/>
-      <c r="T9" s="176"/>
-      <c r="U9" s="177"/>
+      <c r="S9" s="185"/>
+      <c r="T9" s="185"/>
+      <c r="U9" s="186"/>
       <c r="V9" s="42"/>
-      <c r="W9" s="174" t="s">
+      <c r="W9" s="183" t="s">
         <v>517</v>
       </c>
-      <c r="X9" s="174"/>
+      <c r="X9" s="183"/>
       <c r="Y9" s="42"/>
       <c r="Z9" s="43" t="s">
         <v>24</v>
@@ -11109,17 +11064,17 @@
         <v>25</v>
       </c>
       <c r="AC9" s="44"/>
-      <c r="AD9" s="172" t="s">
+      <c r="AD9" s="181" t="s">
         <v>26</v>
       </c>
-      <c r="AE9" s="172"/>
-      <c r="AF9" s="172"/>
+      <c r="AE9" s="181"/>
+      <c r="AF9" s="181"/>
       <c r="AG9" s="42"/>
-      <c r="AH9" s="166" t="s">
+      <c r="AH9" s="175" t="s">
         <v>15</v>
       </c>
-      <c r="AI9" s="167"/>
-      <c r="AJ9" s="168"/>
+      <c r="AI9" s="176"/>
+      <c r="AJ9" s="177"/>
     </row>
     <row r="10" spans="1:1026" ht="13" hidden="1" customHeight="1">
       <c r="A10" s="46" t="s">
@@ -12434,10 +12389,10 @@
         <v>546</v>
       </c>
       <c r="D15" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E15" s="84" t="s">
-        <v>150</v>
+        <v>211</v>
       </c>
       <c r="F15" s="82" t="s">
         <v>564</v>
@@ -12448,7 +12403,7 @@
       <c r="H15" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="181" t="s">
+      <c r="I15" s="169" t="s">
         <v>162</v>
       </c>
       <c r="J15" s="104" t="s">
@@ -12465,13 +12420,13 @@
       </c>
       <c r="N15" s="87"/>
       <c r="O15" s="88" t="s">
-        <v>654</v>
+        <v>637</v>
       </c>
       <c r="P15" s="107" t="s">
         <v>96</v>
       </c>
       <c r="Q15" s="54"/>
-      <c r="R15" s="110"/>
+      <c r="R15" s="169"/>
       <c r="S15" s="138"/>
       <c r="T15" s="82"/>
       <c r="U15" s="89"/>
@@ -12480,10 +12435,10 @@
       <c r="X15" s="108"/>
       <c r="Y15" s="90"/>
       <c r="Z15" s="109" t="s">
-        <v>655</v>
+        <v>638</v>
       </c>
       <c r="AA15" s="92"/>
-      <c r="AB15" s="181" t="s">
+      <c r="AB15" s="169" t="s">
         <v>122</v>
       </c>
       <c r="AC15" s="92"/>
@@ -12498,13 +12453,13 @@
       </c>
       <c r="AG15" s="61"/>
       <c r="AH15" s="88" t="s">
-        <v>657</v>
+        <v>640</v>
       </c>
       <c r="AI15" s="110">
         <v>5</v>
       </c>
-      <c r="AJ15" s="184" t="s">
-        <v>656</v>
+      <c r="AJ15" s="172" t="s">
+        <v>639</v>
       </c>
       <c r="AK15"/>
       <c r="AL15"/>
@@ -13508,7 +13463,7 @@
         <v>546</v>
       </c>
       <c r="D16" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E16" s="84" t="s">
         <v>130</v>
@@ -13522,7 +13477,7 @@
       <c r="H16" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="I16" s="182" t="s">
+      <c r="I16" s="170" t="s">
         <v>104</v>
       </c>
       <c r="J16" s="104" t="s">
@@ -13541,7 +13496,7 @@
       <c r="O16" s="88"/>
       <c r="P16" s="107"/>
       <c r="Q16" s="54"/>
-      <c r="R16" s="110"/>
+      <c r="R16" s="169"/>
       <c r="S16" s="138"/>
       <c r="T16" s="93"/>
       <c r="U16" s="94"/>
@@ -14562,21 +14517,21 @@
         <v>546</v>
       </c>
       <c r="D17" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E17" s="84" t="s">
         <v>135</v>
       </c>
       <c r="F17" s="82" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="G17" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H17" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I17" s="181" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="169" t="s">
         <v>114</v>
       </c>
       <c r="J17" s="104" t="s">
@@ -14595,7 +14550,7 @@
       <c r="O17" s="88"/>
       <c r="P17" s="107"/>
       <c r="Q17" s="54"/>
-      <c r="R17" s="110"/>
+      <c r="R17" s="169"/>
       <c r="S17" s="138"/>
       <c r="T17" s="93"/>
       <c r="U17" s="94"/>
@@ -15616,13 +15571,13 @@
         <v>546</v>
       </c>
       <c r="D18" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E18" s="84" t="s">
         <v>111</v>
       </c>
       <c r="F18" s="82" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
       <c r="G18" s="85" t="s">
         <v>112</v>
@@ -15630,7 +15585,7 @@
       <c r="H18" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="I18" s="182" t="s">
+      <c r="I18" s="170" t="s">
         <v>120</v>
       </c>
       <c r="J18" s="104" t="s">
@@ -15649,7 +15604,7 @@
       <c r="O18" s="88"/>
       <c r="P18" s="107"/>
       <c r="Q18" s="54"/>
-      <c r="R18" s="110"/>
+      <c r="R18" s="169"/>
       <c r="S18" s="138"/>
       <c r="T18" s="93"/>
       <c r="U18" s="94"/>
@@ -16670,21 +16625,21 @@
         <v>546</v>
       </c>
       <c r="D19" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E19" s="84" t="s">
         <v>531</v>
       </c>
       <c r="F19" s="82" t="s">
-        <v>612</v>
+        <v>603</v>
       </c>
       <c r="G19" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H19" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I19" s="181" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="169" t="s">
         <v>126</v>
       </c>
       <c r="J19" s="104" t="s">
@@ -16703,7 +16658,7 @@
       <c r="O19" s="88"/>
       <c r="P19" s="107"/>
       <c r="Q19" s="54"/>
-      <c r="R19" s="110"/>
+      <c r="R19" s="169"/>
       <c r="S19" s="138"/>
       <c r="T19" s="93"/>
       <c r="U19" s="94"/>
@@ -17724,22 +17679,22 @@
         <v>546</v>
       </c>
       <c r="D20" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E20" s="84" t="s">
         <v>140</v>
       </c>
       <c r="F20" s="82" t="s">
-        <v>613</v>
+        <v>604</v>
       </c>
       <c r="G20" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H20" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I20" s="183" t="s">
-        <v>132</v>
+        <v>91</v>
+      </c>
+      <c r="I20" s="171" t="s">
+        <v>126</v>
       </c>
       <c r="J20" s="104" t="s">
         <v>121</v>
@@ -17757,7 +17712,7 @@
       <c r="O20" s="88"/>
       <c r="P20" s="107"/>
       <c r="Q20" s="54"/>
-      <c r="R20" s="110"/>
+      <c r="R20" s="169"/>
       <c r="S20" s="138"/>
       <c r="T20" s="93"/>
       <c r="U20" s="94"/>
@@ -18778,21 +18733,21 @@
         <v>546</v>
       </c>
       <c r="D21" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E21" s="84" t="s">
         <v>518</v>
       </c>
       <c r="F21" s="82" t="s">
-        <v>614</v>
+        <v>605</v>
       </c>
       <c r="G21" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H21" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I21" s="183" t="s">
+        <v>91</v>
+      </c>
+      <c r="I21" s="171" t="s">
         <v>137</v>
       </c>
       <c r="J21" s="104" t="s">
@@ -18811,7 +18766,7 @@
       <c r="O21" s="88"/>
       <c r="P21" s="107"/>
       <c r="Q21" s="54"/>
-      <c r="R21" s="110"/>
+      <c r="R21" s="169"/>
       <c r="S21" s="138"/>
       <c r="T21" s="93"/>
       <c r="U21" s="94"/>
@@ -19832,21 +19787,21 @@
         <v>546</v>
       </c>
       <c r="D22" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E22" s="84" t="s">
         <v>521</v>
       </c>
       <c r="F22" s="82" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="G22" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H22" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I22" s="181" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" s="169" t="s">
         <v>142</v>
       </c>
       <c r="J22" s="104" t="s">
@@ -19865,7 +19820,7 @@
       <c r="O22" s="88"/>
       <c r="P22" s="107"/>
       <c r="Q22" s="54"/>
-      <c r="R22" s="110"/>
+      <c r="R22" s="169"/>
       <c r="S22" s="138"/>
       <c r="T22" s="93"/>
       <c r="U22" s="94"/>
@@ -20886,21 +20841,21 @@
         <v>546</v>
       </c>
       <c r="D23" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E23" s="84" t="s">
         <v>522</v>
       </c>
       <c r="F23" s="82" t="s">
-        <v>616</v>
+        <v>607</v>
       </c>
       <c r="G23" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H23" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I23" s="181" t="s">
+        <v>91</v>
+      </c>
+      <c r="I23" s="169" t="s">
         <v>147</v>
       </c>
       <c r="J23" s="104" t="s">
@@ -20919,7 +20874,7 @@
       <c r="O23" s="88"/>
       <c r="P23" s="107"/>
       <c r="Q23" s="54"/>
-      <c r="R23" s="110"/>
+      <c r="R23" s="169"/>
       <c r="S23" s="138"/>
       <c r="T23" s="93"/>
       <c r="U23" s="94"/>
@@ -21940,21 +21895,21 @@
         <v>546</v>
       </c>
       <c r="D24" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E24" s="84" t="s">
         <v>523</v>
       </c>
       <c r="F24" s="82" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
       <c r="G24" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H24" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I24" s="181" t="s">
+        <v>91</v>
+      </c>
+      <c r="I24" s="169" t="s">
         <v>152</v>
       </c>
       <c r="J24" s="104" t="s">
@@ -21973,7 +21928,7 @@
       <c r="O24" s="88"/>
       <c r="P24" s="107"/>
       <c r="Q24" s="54"/>
-      <c r="R24" s="110"/>
+      <c r="R24" s="169"/>
       <c r="S24" s="138"/>
       <c r="T24" s="93"/>
       <c r="U24" s="94"/>
@@ -22994,21 +22949,21 @@
         <v>546</v>
       </c>
       <c r="D25" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E25" s="84" t="s">
         <v>524</v>
       </c>
       <c r="F25" s="82" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
       <c r="G25" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H25" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I25" s="181" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="169" t="s">
         <v>157</v>
       </c>
       <c r="J25" s="104" t="s">
@@ -23027,7 +22982,7 @@
       <c r="O25" s="88"/>
       <c r="P25" s="107"/>
       <c r="Q25" s="54"/>
-      <c r="R25" s="110"/>
+      <c r="R25" s="169"/>
       <c r="S25" s="138"/>
       <c r="T25" s="93"/>
       <c r="U25" s="94"/>
@@ -24048,21 +24003,21 @@
         <v>546</v>
       </c>
       <c r="D26" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E26" s="84" t="s">
         <v>525</v>
       </c>
       <c r="F26" s="82" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
       <c r="G26" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H26" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I26" s="181" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" s="169" t="s">
         <v>92</v>
       </c>
       <c r="J26" s="104" t="s">
@@ -24081,7 +24036,7 @@
       <c r="O26" s="88"/>
       <c r="P26" s="107"/>
       <c r="Q26" s="54"/>
-      <c r="R26" s="110"/>
+      <c r="R26" s="169"/>
       <c r="S26" s="138"/>
       <c r="T26" s="93"/>
       <c r="U26" s="94"/>
@@ -25102,21 +25057,21 @@
         <v>546</v>
       </c>
       <c r="D27" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E27" s="84" t="s">
         <v>526</v>
       </c>
       <c r="F27" s="82" t="s">
-        <v>620</v>
+        <v>611</v>
       </c>
       <c r="G27" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H27" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I27" s="181" t="s">
+        <v>91</v>
+      </c>
+      <c r="I27" s="169" t="s">
         <v>167</v>
       </c>
       <c r="J27" s="104" t="s">
@@ -25135,7 +25090,7 @@
       <c r="O27" s="88"/>
       <c r="P27" s="107"/>
       <c r="Q27" s="54"/>
-      <c r="R27" s="110"/>
+      <c r="R27" s="169"/>
       <c r="S27" s="138"/>
       <c r="T27" s="93"/>
       <c r="U27" s="94"/>
@@ -25166,22 +25121,22 @@
         <v>546</v>
       </c>
       <c r="D28" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E28" s="84" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="F28" s="82" t="s">
-        <v>621</v>
+        <v>612</v>
       </c>
       <c r="G28" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H28" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I28" s="181" t="s">
-        <v>172</v>
+        <v>91</v>
+      </c>
+      <c r="I28" s="169" t="s">
+        <v>132</v>
       </c>
       <c r="J28" s="104" t="s">
         <v>121</v>
@@ -25199,7 +25154,7 @@
       <c r="O28" s="88"/>
       <c r="P28" s="107"/>
       <c r="Q28" s="54"/>
-      <c r="R28" s="110"/>
+      <c r="R28" s="169"/>
       <c r="S28" s="138"/>
       <c r="T28" s="93"/>
       <c r="U28" s="94"/>
@@ -25209,7 +25164,9 @@
       <c r="Y28" s="90"/>
       <c r="Z28" s="109"/>
       <c r="AA28" s="92"/>
-      <c r="AB28" s="91"/>
+      <c r="AB28" s="169" t="s">
+        <v>95</v>
+      </c>
       <c r="AC28" s="92"/>
       <c r="AD28" s="112"/>
       <c r="AE28" s="112"/>
@@ -26220,21 +26177,23 @@
         <v>546</v>
       </c>
       <c r="D29" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E29" s="84" t="s">
         <v>155</v>
       </c>
       <c r="F29" s="82" t="s">
-        <v>622</v>
+        <v>613</v>
       </c>
       <c r="G29" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H29" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I29" s="179"/>
+        <v>91</v>
+      </c>
+      <c r="I29" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J29" s="104" t="s">
         <v>121</v>
       </c>
@@ -26251,7 +26210,7 @@
       <c r="O29" s="88"/>
       <c r="P29" s="107"/>
       <c r="Q29" s="54"/>
-      <c r="R29" s="110"/>
+      <c r="R29" s="169"/>
       <c r="S29" s="138"/>
       <c r="T29" s="93"/>
       <c r="U29" s="94"/>
@@ -26261,8 +26220,8 @@
       <c r="Y29" s="90"/>
       <c r="Z29" s="109"/>
       <c r="AA29" s="92"/>
-      <c r="AB29" s="181" t="s">
-        <v>95</v>
+      <c r="AB29" s="169" t="s">
+        <v>107</v>
       </c>
       <c r="AC29" s="92"/>
       <c r="AD29" s="112"/>
@@ -27274,21 +27233,23 @@
         <v>546</v>
       </c>
       <c r="D30" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E30" s="84" t="s">
         <v>160</v>
       </c>
       <c r="F30" s="82" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
       <c r="G30" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H30" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I30" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I30" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J30" s="104" t="s">
         <v>121</v>
       </c>
@@ -27305,7 +27266,7 @@
       <c r="O30" s="88"/>
       <c r="P30" s="107"/>
       <c r="Q30" s="54"/>
-      <c r="R30" s="110"/>
+      <c r="R30" s="169"/>
       <c r="S30" s="138"/>
       <c r="T30" s="93"/>
       <c r="U30" s="94"/>
@@ -27315,8 +27276,8 @@
       <c r="Y30" s="90"/>
       <c r="Z30" s="109"/>
       <c r="AA30" s="92"/>
-      <c r="AB30" s="181" t="s">
-        <v>107</v>
+      <c r="AB30" s="91" t="s">
+        <v>116</v>
       </c>
       <c r="AC30" s="92"/>
       <c r="AD30" s="112"/>
@@ -28328,21 +28289,23 @@
         <v>546</v>
       </c>
       <c r="D31" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E31" s="84" t="s">
         <v>165</v>
       </c>
       <c r="F31" s="82" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
       <c r="G31" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H31" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I31" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I31" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J31" s="104" t="s">
         <v>121</v>
       </c>
@@ -28359,7 +28322,7 @@
       <c r="O31" s="88"/>
       <c r="P31" s="107"/>
       <c r="Q31" s="54"/>
-      <c r="R31" s="110"/>
+      <c r="R31" s="169"/>
       <c r="S31" s="138"/>
       <c r="T31" s="93"/>
       <c r="U31" s="94"/>
@@ -29382,21 +29345,23 @@
         <v>546</v>
       </c>
       <c r="D32" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E32" s="84" t="s">
         <v>170</v>
       </c>
       <c r="F32" s="82" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
       <c r="G32" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H32" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I32" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I32" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J32" s="104" t="s">
         <v>121</v>
       </c>
@@ -29413,7 +29378,7 @@
       <c r="O32" s="88"/>
       <c r="P32" s="107"/>
       <c r="Q32" s="54"/>
-      <c r="R32" s="110"/>
+      <c r="R32" s="169"/>
       <c r="S32" s="138"/>
       <c r="T32" s="93"/>
       <c r="U32" s="94"/>
@@ -30436,21 +30401,23 @@
         <v>546</v>
       </c>
       <c r="D33" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E33" s="84" t="s">
         <v>175</v>
       </c>
       <c r="F33" s="82" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
       <c r="G33" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H33" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I33" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I33" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J33" s="104" t="s">
         <v>121</v>
       </c>
@@ -30467,7 +30434,7 @@
       <c r="O33" s="88"/>
       <c r="P33" s="107"/>
       <c r="Q33" s="54"/>
-      <c r="R33" s="110"/>
+      <c r="R33" s="169"/>
       <c r="S33" s="138"/>
       <c r="T33" s="93"/>
       <c r="U33" s="94"/>
@@ -31490,21 +31457,23 @@
         <v>546</v>
       </c>
       <c r="D34" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E34" s="84" t="s">
         <v>179</v>
       </c>
       <c r="F34" s="82" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
       <c r="G34" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H34" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I34" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I34" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J34" s="104" t="s">
         <v>121</v>
       </c>
@@ -31521,7 +31490,7 @@
       <c r="O34" s="88"/>
       <c r="P34" s="107"/>
       <c r="Q34" s="54"/>
-      <c r="R34" s="110"/>
+      <c r="R34" s="169"/>
       <c r="S34" s="138"/>
       <c r="T34" s="93"/>
       <c r="U34" s="94"/>
@@ -32544,21 +32513,23 @@
         <v>546</v>
       </c>
       <c r="D35" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E35" s="84" t="s">
         <v>183</v>
       </c>
       <c r="F35" s="82" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
       <c r="G35" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H35" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I35" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I35" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J35" s="104" t="s">
         <v>121</v>
       </c>
@@ -32575,7 +32546,7 @@
       <c r="O35" s="88"/>
       <c r="P35" s="107"/>
       <c r="Q35" s="54"/>
-      <c r="R35" s="110"/>
+      <c r="R35" s="169"/>
       <c r="S35" s="138"/>
       <c r="T35" s="93"/>
       <c r="U35" s="94"/>
@@ -33598,21 +33569,23 @@
         <v>546</v>
       </c>
       <c r="D36" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E36" s="84" t="s">
         <v>187</v>
       </c>
       <c r="F36" s="82" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
       <c r="G36" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H36" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I36" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I36" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J36" s="104" t="s">
         <v>121</v>
       </c>
@@ -33629,7 +33602,7 @@
       <c r="O36" s="88"/>
       <c r="P36" s="107"/>
       <c r="Q36" s="54"/>
-      <c r="R36" s="110"/>
+      <c r="R36" s="169"/>
       <c r="S36" s="138"/>
       <c r="T36" s="93"/>
       <c r="U36" s="94"/>
@@ -33662,21 +33635,23 @@
         <v>546</v>
       </c>
       <c r="D37" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E37" s="84" t="s">
         <v>191</v>
       </c>
       <c r="F37" s="82" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
       <c r="G37" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H37" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I37" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I37" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J37" s="104" t="s">
         <v>121</v>
       </c>
@@ -33693,7 +33668,7 @@
       <c r="O37" s="88"/>
       <c r="P37" s="107"/>
       <c r="Q37" s="54"/>
-      <c r="R37" s="110"/>
+      <c r="R37" s="173"/>
       <c r="S37" s="138"/>
       <c r="T37" s="93"/>
       <c r="U37" s="94"/>
@@ -33726,21 +33701,23 @@
         <v>546</v>
       </c>
       <c r="D38" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E38" s="84" t="s">
         <v>195</v>
       </c>
       <c r="F38" s="82" t="s">
-        <v>631</v>
+        <v>622</v>
       </c>
       <c r="G38" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H38" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I38" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I38" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J38" s="104" t="s">
         <v>121</v>
       </c>
@@ -33757,7 +33734,7 @@
       <c r="O38" s="88"/>
       <c r="P38" s="107"/>
       <c r="Q38" s="54"/>
-      <c r="R38" s="110"/>
+      <c r="R38" s="169"/>
       <c r="S38" s="138"/>
       <c r="T38" s="93"/>
       <c r="U38" s="94"/>
@@ -33790,21 +33767,23 @@
         <v>546</v>
       </c>
       <c r="D39" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E39" s="84" t="s">
         <v>199</v>
       </c>
       <c r="F39" s="82" t="s">
-        <v>632</v>
+        <v>623</v>
       </c>
       <c r="G39" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H39" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I39" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I39" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J39" s="104" t="s">
         <v>121</v>
       </c>
@@ -33821,7 +33800,7 @@
       <c r="O39" s="88"/>
       <c r="P39" s="107"/>
       <c r="Q39" s="54"/>
-      <c r="R39" s="110"/>
+      <c r="R39" s="169"/>
       <c r="S39" s="138"/>
       <c r="T39" s="93"/>
       <c r="U39" s="94"/>
@@ -34844,21 +34823,23 @@
         <v>546</v>
       </c>
       <c r="D40" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E40" s="84" t="s">
         <v>203</v>
       </c>
       <c r="F40" s="82" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
       <c r="G40" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H40" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I40" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I40" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J40" s="104" t="s">
         <v>121</v>
       </c>
@@ -34875,7 +34856,7 @@
       <c r="O40" s="88"/>
       <c r="P40" s="107"/>
       <c r="Q40" s="54"/>
-      <c r="R40" s="110"/>
+      <c r="R40" s="169"/>
       <c r="S40" s="138"/>
       <c r="T40" s="93"/>
       <c r="U40" s="94"/>
@@ -35898,21 +35879,23 @@
         <v>546</v>
       </c>
       <c r="D41" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E41" s="84" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
       <c r="F41" s="82" t="s">
-        <v>634</v>
+        <v>625</v>
       </c>
       <c r="G41" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H41" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I41" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I41" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J41" s="104" t="s">
         <v>121</v>
       </c>
@@ -35929,7 +35912,7 @@
       <c r="O41" s="88"/>
       <c r="P41" s="107"/>
       <c r="Q41" s="54"/>
-      <c r="R41" s="110"/>
+      <c r="R41" s="169"/>
       <c r="S41" s="138"/>
       <c r="T41" s="93"/>
       <c r="U41" s="94"/>
@@ -36952,21 +36935,23 @@
         <v>546</v>
       </c>
       <c r="D42" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E42" s="84" t="s">
         <v>215</v>
       </c>
       <c r="F42" s="82" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
       <c r="G42" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H42" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I42" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I42" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J42" s="104" t="s">
         <v>121</v>
       </c>
@@ -36983,7 +36968,7 @@
       <c r="O42" s="88"/>
       <c r="P42" s="107"/>
       <c r="Q42" s="54"/>
-      <c r="R42" s="110"/>
+      <c r="R42" s="169"/>
       <c r="S42" s="138"/>
       <c r="T42" s="93"/>
       <c r="U42" s="94"/>
@@ -36991,7 +36976,9 @@
       <c r="W42" s="95"/>
       <c r="X42" s="108"/>
       <c r="Y42" s="90"/>
-      <c r="Z42" s="109"/>
+      <c r="Z42" s="109" t="s">
+        <v>638</v>
+      </c>
       <c r="AA42" s="92"/>
       <c r="AB42" s="91" t="s">
         <v>116</v>
@@ -38006,21 +37993,23 @@
         <v>546</v>
       </c>
       <c r="D43" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E43" s="84" t="s">
         <v>219</v>
       </c>
       <c r="F43" s="82" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="G43" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H43" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I43" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I43" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J43" s="104" t="s">
         <v>121</v>
       </c>
@@ -38037,7 +38026,7 @@
       <c r="O43" s="88"/>
       <c r="P43" s="107"/>
       <c r="Q43" s="54"/>
-      <c r="R43" s="110"/>
+      <c r="R43" s="169"/>
       <c r="S43" s="138"/>
       <c r="T43" s="93"/>
       <c r="U43" s="94"/>
@@ -38045,7 +38034,9 @@
       <c r="W43" s="95"/>
       <c r="X43" s="108"/>
       <c r="Y43" s="90"/>
-      <c r="Z43" s="109"/>
+      <c r="Z43" s="109" t="s">
+        <v>638</v>
+      </c>
       <c r="AA43" s="92"/>
       <c r="AB43" s="91" t="s">
         <v>116</v>
@@ -39060,21 +39051,23 @@
         <v>546</v>
       </c>
       <c r="D44" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E44" s="84" t="s">
         <v>222</v>
       </c>
       <c r="F44" s="82" t="s">
-        <v>637</v>
+        <v>628</v>
       </c>
       <c r="G44" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H44" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I44" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I44" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J44" s="104" t="s">
         <v>121</v>
       </c>
@@ -39091,7 +39084,7 @@
       <c r="O44" s="88"/>
       <c r="P44" s="107"/>
       <c r="Q44" s="54"/>
-      <c r="R44" s="110"/>
+      <c r="R44" s="169"/>
       <c r="S44" s="138"/>
       <c r="T44" s="93"/>
       <c r="U44" s="94"/>
@@ -39099,7 +39092,9 @@
       <c r="W44" s="95"/>
       <c r="X44" s="108"/>
       <c r="Y44" s="90"/>
-      <c r="Z44" s="109"/>
+      <c r="Z44" s="109" t="s">
+        <v>638</v>
+      </c>
       <c r="AA44" s="92"/>
       <c r="AB44" s="91" t="s">
         <v>116</v>
@@ -40114,21 +40109,23 @@
         <v>546</v>
       </c>
       <c r="D45" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E45" s="84" t="s">
         <v>226</v>
       </c>
       <c r="F45" s="82" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
       <c r="G45" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H45" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I45" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I45" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J45" s="104" t="s">
         <v>121</v>
       </c>
@@ -40145,7 +40142,7 @@
       <c r="O45" s="88"/>
       <c r="P45" s="107"/>
       <c r="Q45" s="54"/>
-      <c r="R45" s="110"/>
+      <c r="R45" s="169"/>
       <c r="S45" s="138"/>
       <c r="T45" s="93"/>
       <c r="U45" s="94"/>
@@ -40153,7 +40150,9 @@
       <c r="W45" s="95"/>
       <c r="X45" s="108"/>
       <c r="Y45" s="90"/>
-      <c r="Z45" s="109"/>
+      <c r="Z45" s="109" t="s">
+        <v>638</v>
+      </c>
       <c r="AA45" s="92"/>
       <c r="AB45" s="91" t="s">
         <v>116</v>
@@ -41168,21 +41167,23 @@
         <v>546</v>
       </c>
       <c r="D46" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E46" s="84" t="s">
         <v>230</v>
       </c>
       <c r="F46" s="82" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
       <c r="G46" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H46" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I46" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I46" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J46" s="104" t="s">
         <v>121</v>
       </c>
@@ -41199,7 +41200,7 @@
       <c r="O46" s="88"/>
       <c r="P46" s="107"/>
       <c r="Q46" s="54"/>
-      <c r="R46" s="110"/>
+      <c r="R46" s="169"/>
       <c r="S46" s="138"/>
       <c r="T46" s="93"/>
       <c r="U46" s="94"/>
@@ -41207,7 +41208,9 @@
       <c r="W46" s="95"/>
       <c r="X46" s="108"/>
       <c r="Y46" s="90"/>
-      <c r="Z46" s="109"/>
+      <c r="Z46" s="109" t="s">
+        <v>638</v>
+      </c>
       <c r="AA46" s="92"/>
       <c r="AB46" s="91" t="s">
         <v>116</v>
@@ -42222,21 +42225,23 @@
         <v>546</v>
       </c>
       <c r="D47" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E47" s="84" t="s">
         <v>234</v>
       </c>
       <c r="F47" s="82" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
       <c r="G47" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H47" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I47" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I47" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J47" s="104" t="s">
         <v>121</v>
       </c>
@@ -42253,7 +42258,7 @@
       <c r="O47" s="88"/>
       <c r="P47" s="107"/>
       <c r="Q47" s="54"/>
-      <c r="R47" s="110"/>
+      <c r="R47" s="169"/>
       <c r="S47" s="138"/>
       <c r="T47" s="93"/>
       <c r="U47" s="94"/>
@@ -42261,7 +42266,9 @@
       <c r="W47" s="95"/>
       <c r="X47" s="108"/>
       <c r="Y47" s="90"/>
-      <c r="Z47" s="109"/>
+      <c r="Z47" s="109" t="s">
+        <v>638</v>
+      </c>
       <c r="AA47" s="92"/>
       <c r="AB47" s="91" t="s">
         <v>116</v>
@@ -43276,21 +43283,23 @@
         <v>546</v>
       </c>
       <c r="D48" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E48" s="84" t="s">
         <v>238</v>
       </c>
       <c r="F48" s="82" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
       <c r="G48" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H48" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I48" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I48" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J48" s="104" t="s">
         <v>121</v>
       </c>
@@ -43307,7 +43316,7 @@
       <c r="O48" s="88"/>
       <c r="P48" s="107"/>
       <c r="Q48" s="54"/>
-      <c r="R48" s="110"/>
+      <c r="R48" s="169"/>
       <c r="S48" s="138"/>
       <c r="T48" s="93"/>
       <c r="U48" s="94"/>
@@ -43315,7 +43324,9 @@
       <c r="W48" s="95"/>
       <c r="X48" s="108"/>
       <c r="Y48" s="90"/>
-      <c r="Z48" s="109"/>
+      <c r="Z48" s="109" t="s">
+        <v>638</v>
+      </c>
       <c r="AA48" s="92"/>
       <c r="AB48" s="91" t="s">
         <v>116</v>
@@ -44330,21 +44341,23 @@
         <v>546</v>
       </c>
       <c r="D49" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E49" s="84" t="s">
         <v>242</v>
       </c>
       <c r="F49" s="82" t="s">
-        <v>642</v>
+        <v>633</v>
       </c>
       <c r="G49" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H49" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I49" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I49" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J49" s="104" t="s">
         <v>121</v>
       </c>
@@ -44361,7 +44374,7 @@
       <c r="O49" s="88"/>
       <c r="P49" s="107"/>
       <c r="Q49" s="54"/>
-      <c r="R49" s="110"/>
+      <c r="R49" s="169"/>
       <c r="S49" s="138"/>
       <c r="T49" s="93"/>
       <c r="U49" s="94"/>
@@ -44369,7 +44382,9 @@
       <c r="W49" s="95"/>
       <c r="X49" s="108"/>
       <c r="Y49" s="90"/>
-      <c r="Z49" s="109"/>
+      <c r="Z49" s="109" t="s">
+        <v>638</v>
+      </c>
       <c r="AA49" s="92"/>
       <c r="AB49" s="91" t="s">
         <v>116</v>
@@ -45384,21 +45399,23 @@
         <v>546</v>
       </c>
       <c r="D50" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E50" s="84" t="s">
         <v>246</v>
       </c>
       <c r="F50" s="82" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
       <c r="G50" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H50" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I50" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I50" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J50" s="104" t="s">
         <v>121</v>
       </c>
@@ -45415,7 +45432,7 @@
       <c r="O50" s="88"/>
       <c r="P50" s="107"/>
       <c r="Q50" s="54"/>
-      <c r="R50" s="110"/>
+      <c r="R50" s="169"/>
       <c r="S50" s="138"/>
       <c r="T50" s="93"/>
       <c r="U50" s="94"/>
@@ -45423,7 +45440,9 @@
       <c r="W50" s="95"/>
       <c r="X50" s="108"/>
       <c r="Y50" s="90"/>
-      <c r="Z50" s="109"/>
+      <c r="Z50" s="109" t="s">
+        <v>638</v>
+      </c>
       <c r="AA50" s="92"/>
       <c r="AB50" s="91" t="s">
         <v>116</v>
@@ -45448,21 +45467,23 @@
         <v>546</v>
       </c>
       <c r="D51" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E51" s="84" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F51" s="82" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
       <c r="G51" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H51" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I51" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I51" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J51" s="104" t="s">
         <v>121</v>
       </c>
@@ -45479,7 +45500,7 @@
       <c r="O51" s="88"/>
       <c r="P51" s="107"/>
       <c r="Q51" s="54"/>
-      <c r="R51" s="110"/>
+      <c r="R51" s="170"/>
       <c r="S51" s="138"/>
       <c r="T51" s="93"/>
       <c r="U51" s="94"/>
@@ -45487,9 +45508,13 @@
       <c r="W51" s="95"/>
       <c r="X51" s="108"/>
       <c r="Y51" s="90"/>
-      <c r="Z51" s="109"/>
+      <c r="Z51" s="109" t="s">
+        <v>638</v>
+      </c>
       <c r="AA51" s="92"/>
-      <c r="AB51" s="91"/>
+      <c r="AB51" s="91" t="s">
+        <v>116</v>
+      </c>
       <c r="AC51" s="92"/>
       <c r="AD51" s="112"/>
       <c r="AE51" s="112"/>
@@ -46500,21 +46525,23 @@
         <v>546</v>
       </c>
       <c r="D52" s="84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E52" s="84" t="s">
-        <v>393</v>
+        <v>246</v>
       </c>
       <c r="F52" s="82" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
       <c r="G52" s="85" t="s">
         <v>112</v>
       </c>
       <c r="H52" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I52" s="103"/>
+        <v>91</v>
+      </c>
+      <c r="I52" s="169" t="s">
+        <v>92</v>
+      </c>
       <c r="J52" s="104" t="s">
         <v>121</v>
       </c>
@@ -46531,7 +46558,7 @@
       <c r="O52" s="88"/>
       <c r="P52" s="107"/>
       <c r="Q52" s="54"/>
-      <c r="R52" s="110"/>
+      <c r="R52" s="174"/>
       <c r="S52" s="138"/>
       <c r="T52" s="93"/>
       <c r="U52" s="94"/>
@@ -46539,9 +46566,13 @@
       <c r="W52" s="95"/>
       <c r="X52" s="108"/>
       <c r="Y52" s="90"/>
-      <c r="Z52" s="109"/>
+      <c r="Z52" s="109" t="s">
+        <v>638</v>
+      </c>
       <c r="AA52" s="92"/>
-      <c r="AB52" s="91"/>
+      <c r="AB52" s="91" t="s">
+        <v>116</v>
+      </c>
       <c r="AC52" s="92"/>
       <c r="AD52" s="112"/>
       <c r="AE52" s="112"/>
@@ -47542,48 +47573,24 @@
       <c r="AML52"/>
     </row>
     <row r="53" spans="1:1026" ht="25" customHeight="1">
-      <c r="A53" s="82" t="s">
-        <v>602</v>
-      </c>
-      <c r="B53" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="84" t="s">
-        <v>546</v>
-      </c>
-      <c r="D53" s="84" t="s">
-        <v>550</v>
-      </c>
-      <c r="E53" s="84" t="s">
-        <v>258</v>
-      </c>
-      <c r="F53" s="82" t="s">
-        <v>646</v>
-      </c>
-      <c r="G53" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="H53" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I53" s="103"/>
-      <c r="J53" s="104" t="s">
-        <v>121</v>
-      </c>
-      <c r="K53" s="105" t="s">
-        <v>103</v>
-      </c>
-      <c r="L53" s="105">
-        <v>1</v>
-      </c>
-      <c r="M53" s="106" t="s">
-        <v>99</v>
-      </c>
+      <c r="A53" s="82"/>
+      <c r="B53" s="83"/>
+      <c r="C53" s="84"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="84"/>
+      <c r="F53" s="82"/>
+      <c r="G53" s="85"/>
+      <c r="H53" s="86"/>
+      <c r="I53" s="169"/>
+      <c r="J53" s="104"/>
+      <c r="K53" s="105"/>
+      <c r="L53" s="105"/>
+      <c r="M53" s="106"/>
       <c r="N53" s="87"/>
       <c r="O53" s="88"/>
       <c r="P53" s="107"/>
       <c r="Q53" s="54"/>
-      <c r="R53" s="110"/>
+      <c r="R53" s="174"/>
       <c r="S53" s="138"/>
       <c r="T53" s="93"/>
       <c r="U53" s="94"/>
@@ -48594,48 +48601,24 @@
       <c r="AML53"/>
     </row>
     <row r="54" spans="1:1026" ht="25" customHeight="1">
-      <c r="A54" s="82" t="s">
-        <v>603</v>
-      </c>
-      <c r="B54" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="C54" s="84" t="s">
-        <v>546</v>
-      </c>
-      <c r="D54" s="84" t="s">
-        <v>550</v>
-      </c>
-      <c r="E54" s="84" t="s">
-        <v>262</v>
-      </c>
-      <c r="F54" s="82" t="s">
-        <v>647</v>
-      </c>
-      <c r="G54" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="H54" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I54" s="103"/>
-      <c r="J54" s="104" t="s">
-        <v>121</v>
-      </c>
-      <c r="K54" s="105" t="s">
-        <v>103</v>
-      </c>
-      <c r="L54" s="105">
-        <v>1</v>
-      </c>
-      <c r="M54" s="106" t="s">
-        <v>99</v>
-      </c>
+      <c r="A54" s="82"/>
+      <c r="B54" s="83"/>
+      <c r="C54" s="84"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="84"/>
+      <c r="F54" s="82"/>
+      <c r="G54" s="85"/>
+      <c r="H54" s="86"/>
+      <c r="I54" s="169"/>
+      <c r="J54" s="104"/>
+      <c r="K54" s="105"/>
+      <c r="L54" s="105"/>
+      <c r="M54" s="106"/>
       <c r="N54" s="87"/>
       <c r="O54" s="88"/>
       <c r="P54" s="107"/>
       <c r="Q54" s="54"/>
-      <c r="R54" s="110"/>
+      <c r="R54" s="174"/>
       <c r="S54" s="138"/>
       <c r="T54" s="93"/>
       <c r="U54" s="94"/>
@@ -49646,48 +49629,24 @@
       <c r="AML54"/>
     </row>
     <row r="55" spans="1:1026" ht="25" customHeight="1">
-      <c r="A55" s="82" t="s">
-        <v>604</v>
-      </c>
-      <c r="B55" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="C55" s="84" t="s">
-        <v>546</v>
-      </c>
-      <c r="D55" s="84" t="s">
-        <v>550</v>
-      </c>
-      <c r="E55" s="84" t="s">
-        <v>266</v>
-      </c>
-      <c r="F55" s="82" t="s">
-        <v>648</v>
-      </c>
-      <c r="G55" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="H55" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I55" s="103"/>
-      <c r="J55" s="104" t="s">
-        <v>121</v>
-      </c>
-      <c r="K55" s="105" t="s">
-        <v>103</v>
-      </c>
-      <c r="L55" s="105">
-        <v>1</v>
-      </c>
-      <c r="M55" s="106" t="s">
-        <v>99</v>
-      </c>
+      <c r="A55" s="82"/>
+      <c r="B55" s="83"/>
+      <c r="C55" s="84"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="84"/>
+      <c r="F55" s="82"/>
+      <c r="G55" s="85"/>
+      <c r="H55" s="86"/>
+      <c r="I55" s="169"/>
+      <c r="J55" s="104"/>
+      <c r="K55" s="105"/>
+      <c r="L55" s="105"/>
+      <c r="M55" s="106"/>
       <c r="N55" s="87"/>
       <c r="O55" s="88"/>
       <c r="P55" s="107"/>
       <c r="Q55" s="54"/>
-      <c r="R55" s="110"/>
+      <c r="R55" s="174"/>
       <c r="S55" s="138"/>
       <c r="T55" s="93"/>
       <c r="U55" s="94"/>
@@ -50698,48 +50657,24 @@
       <c r="AML55"/>
     </row>
     <row r="56" spans="1:1026" ht="25" customHeight="1">
-      <c r="A56" s="82" t="s">
-        <v>605</v>
-      </c>
-      <c r="B56" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="C56" s="84" t="s">
-        <v>546</v>
-      </c>
-      <c r="D56" s="84" t="s">
-        <v>550</v>
-      </c>
-      <c r="E56" s="84" t="s">
-        <v>392</v>
-      </c>
-      <c r="F56" s="82" t="s">
-        <v>649</v>
-      </c>
-      <c r="G56" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="H56" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I56" s="103"/>
-      <c r="J56" s="104" t="s">
-        <v>121</v>
-      </c>
-      <c r="K56" s="105" t="s">
-        <v>103</v>
-      </c>
-      <c r="L56" s="105">
-        <v>1</v>
-      </c>
-      <c r="M56" s="106" t="s">
-        <v>99</v>
-      </c>
+      <c r="A56" s="82"/>
+      <c r="B56" s="83"/>
+      <c r="C56" s="84"/>
+      <c r="D56" s="84"/>
+      <c r="E56" s="84"/>
+      <c r="F56" s="82"/>
+      <c r="G56" s="85"/>
+      <c r="H56" s="86"/>
+      <c r="I56" s="169"/>
+      <c r="J56" s="104"/>
+      <c r="K56" s="105"/>
+      <c r="L56" s="105"/>
+      <c r="M56" s="106"/>
       <c r="N56" s="87"/>
       <c r="O56" s="88"/>
       <c r="P56" s="107"/>
       <c r="Q56" s="54"/>
-      <c r="R56" s="110"/>
+      <c r="R56" s="174"/>
       <c r="S56" s="138"/>
       <c r="T56" s="93"/>
       <c r="U56" s="94"/>
@@ -51750,48 +51685,24 @@
       <c r="AML56"/>
     </row>
     <row r="57" spans="1:1026" ht="25" customHeight="1">
-      <c r="A57" s="82" t="s">
-        <v>606</v>
-      </c>
-      <c r="B57" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="C57" s="84" t="s">
-        <v>546</v>
-      </c>
-      <c r="D57" s="84" t="s">
-        <v>550</v>
-      </c>
-      <c r="E57" s="84" t="s">
-        <v>270</v>
-      </c>
-      <c r="F57" s="82" t="s">
-        <v>650</v>
-      </c>
-      <c r="G57" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="H57" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I57" s="103"/>
-      <c r="J57" s="104" t="s">
-        <v>121</v>
-      </c>
-      <c r="K57" s="105" t="s">
-        <v>103</v>
-      </c>
-      <c r="L57" s="105">
-        <v>1</v>
-      </c>
-      <c r="M57" s="106" t="s">
-        <v>99</v>
-      </c>
+      <c r="A57" s="82"/>
+      <c r="B57" s="83"/>
+      <c r="C57" s="84"/>
+      <c r="D57" s="84"/>
+      <c r="E57" s="84"/>
+      <c r="F57" s="82"/>
+      <c r="G57" s="85"/>
+      <c r="H57" s="86"/>
+      <c r="I57" s="169"/>
+      <c r="J57" s="104"/>
+      <c r="K57" s="105"/>
+      <c r="L57" s="105"/>
+      <c r="M57" s="106"/>
       <c r="N57" s="87"/>
       <c r="O57" s="88"/>
       <c r="P57" s="107"/>
       <c r="Q57" s="54"/>
-      <c r="R57" s="110"/>
+      <c r="R57" s="174"/>
       <c r="S57" s="138"/>
       <c r="T57" s="93"/>
       <c r="U57" s="94"/>
@@ -52802,48 +52713,24 @@
       <c r="AML57"/>
     </row>
     <row r="58" spans="1:1026" ht="25" customHeight="1">
-      <c r="A58" s="82" t="s">
-        <v>607</v>
-      </c>
-      <c r="B58" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="C58" s="84" t="s">
-        <v>546</v>
-      </c>
-      <c r="D58" s="84" t="s">
-        <v>550</v>
-      </c>
-      <c r="E58" s="178" t="s">
-        <v>394</v>
-      </c>
-      <c r="F58" s="82" t="s">
-        <v>651</v>
-      </c>
-      <c r="G58" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="H58" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I58" s="103"/>
-      <c r="J58" s="104" t="s">
-        <v>121</v>
-      </c>
-      <c r="K58" s="105" t="s">
-        <v>103</v>
-      </c>
-      <c r="L58" s="105">
-        <v>1</v>
-      </c>
-      <c r="M58" s="106" t="s">
-        <v>99</v>
-      </c>
+      <c r="A58" s="82"/>
+      <c r="B58" s="83"/>
+      <c r="C58" s="84"/>
+      <c r="D58" s="84"/>
+      <c r="E58" s="166"/>
+      <c r="F58" s="82"/>
+      <c r="G58" s="85"/>
+      <c r="H58" s="86"/>
+      <c r="I58" s="169"/>
+      <c r="J58" s="104"/>
+      <c r="K58" s="105"/>
+      <c r="L58" s="105"/>
+      <c r="M58" s="106"/>
       <c r="N58" s="87"/>
       <c r="O58" s="88"/>
       <c r="P58" s="107"/>
       <c r="Q58" s="54"/>
-      <c r="R58" s="110"/>
+      <c r="R58" s="174"/>
       <c r="S58" s="138"/>
       <c r="T58" s="93"/>
       <c r="U58" s="94"/>
@@ -53854,48 +53741,24 @@
       <c r="AML58"/>
     </row>
     <row r="59" spans="1:1026" ht="25" customHeight="1">
-      <c r="A59" s="82" t="s">
-        <v>608</v>
-      </c>
-      <c r="B59" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59" s="84" t="s">
-        <v>546</v>
-      </c>
-      <c r="D59" s="84" t="s">
-        <v>550</v>
-      </c>
-      <c r="E59" s="178" t="s">
-        <v>396</v>
-      </c>
-      <c r="F59" s="82" t="s">
-        <v>652</v>
-      </c>
-      <c r="G59" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="H59" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I59" s="103"/>
-      <c r="J59" s="104" t="s">
-        <v>121</v>
-      </c>
-      <c r="K59" s="105" t="s">
-        <v>103</v>
-      </c>
-      <c r="L59" s="105">
-        <v>1</v>
-      </c>
-      <c r="M59" s="106" t="s">
-        <v>99</v>
-      </c>
+      <c r="A59" s="82"/>
+      <c r="B59" s="83"/>
+      <c r="C59" s="84"/>
+      <c r="D59" s="84"/>
+      <c r="E59" s="166"/>
+      <c r="F59" s="82"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="86"/>
+      <c r="I59" s="169"/>
+      <c r="J59" s="104"/>
+      <c r="K59" s="105"/>
+      <c r="L59" s="105"/>
+      <c r="M59" s="106"/>
       <c r="N59" s="87"/>
       <c r="O59" s="88"/>
       <c r="P59" s="107"/>
       <c r="Q59" s="54"/>
-      <c r="R59" s="110"/>
+      <c r="R59" s="174"/>
       <c r="S59" s="138"/>
       <c r="T59" s="93"/>
       <c r="U59" s="94"/>
@@ -54906,48 +54769,24 @@
       <c r="AML59"/>
     </row>
     <row r="60" spans="1:1026" ht="25" customHeight="1">
-      <c r="A60" s="82" t="s">
-        <v>609</v>
-      </c>
-      <c r="B60" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="C60" s="84" t="s">
-        <v>546</v>
-      </c>
-      <c r="D60" s="84" t="s">
-        <v>550</v>
-      </c>
-      <c r="E60" s="178" t="s">
-        <v>395</v>
-      </c>
-      <c r="F60" s="82" t="s">
-        <v>653</v>
-      </c>
-      <c r="G60" s="85" t="s">
-        <v>112</v>
-      </c>
-      <c r="H60" s="86" t="s">
-        <v>103</v>
-      </c>
-      <c r="I60" s="103"/>
-      <c r="J60" s="104" t="s">
-        <v>121</v>
-      </c>
-      <c r="K60" s="105" t="s">
-        <v>103</v>
-      </c>
-      <c r="L60" s="105">
-        <v>1</v>
-      </c>
-      <c r="M60" s="106" t="s">
-        <v>99</v>
-      </c>
+      <c r="A60" s="82"/>
+      <c r="B60" s="83"/>
+      <c r="C60" s="84"/>
+      <c r="D60" s="84"/>
+      <c r="E60" s="166"/>
+      <c r="F60" s="82"/>
+      <c r="G60" s="85"/>
+      <c r="H60" s="86"/>
+      <c r="I60" s="169"/>
+      <c r="J60" s="104"/>
+      <c r="K60" s="105"/>
+      <c r="L60" s="105"/>
+      <c r="M60" s="106"/>
       <c r="N60" s="87"/>
       <c r="O60" s="88"/>
       <c r="P60" s="107"/>
       <c r="Q60" s="54"/>
-      <c r="R60" s="110"/>
+      <c r="R60" s="174"/>
       <c r="S60" s="138"/>
       <c r="T60" s="93"/>
       <c r="U60" s="94"/>
@@ -55962,7 +55801,7 @@
       <c r="B61" s="83"/>
       <c r="C61" s="84"/>
       <c r="D61" s="84"/>
-      <c r="E61" s="179"/>
+      <c r="E61" s="167"/>
       <c r="F61" s="89"/>
       <c r="G61" s="85"/>
       <c r="H61" s="86"/>
@@ -56990,7 +56829,7 @@
       <c r="B62" s="83"/>
       <c r="C62" s="84"/>
       <c r="D62" s="84"/>
-      <c r="E62" s="179"/>
+      <c r="E62" s="167"/>
       <c r="F62" s="89"/>
       <c r="G62" s="85"/>
       <c r="H62" s="86"/>
@@ -58018,7 +57857,7 @@
       <c r="B63" s="83"/>
       <c r="C63" s="84"/>
       <c r="D63" s="84"/>
-      <c r="E63" s="180"/>
+      <c r="E63" s="168"/>
       <c r="F63" s="89"/>
       <c r="G63" s="85"/>
       <c r="H63" s="86"/>
@@ -58056,7 +57895,7 @@
       <c r="B64" s="83"/>
       <c r="C64" s="84"/>
       <c r="D64" s="84"/>
-      <c r="E64" s="180"/>
+      <c r="E64" s="168"/>
       <c r="F64" s="89"/>
       <c r="G64" s="85"/>
       <c r="H64" s="86"/>
@@ -70787,7 +70626,7 @@
   <dimension ref="A2:AM203"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L5"/>
+      <selection activeCell="N3" sqref="N3:N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
update with newest 1508:22 OF
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.22.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.22.balsamic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F87011C-5CCE-F64D-925D-5D807147AD9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E928A6-0DA1-E045-A5ED-14CE59DF5936}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8080" yWindow="4460" windowWidth="32000" windowHeight="15940" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17360" yWindow="460" windowWidth="21040" windowHeight="21140" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Drop down lists" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="description" localSheetId="2">'Drop down lists'!$D$36</definedName>
+    <definedName name="description" localSheetId="2">'Drop down lists'!$D$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="641">
   <si>
     <t>Document name</t>
   </si>
@@ -1828,9 +1828,6 @@
     <t>This information is optional for RNA analysis</t>
   </si>
   <si>
-    <t>WGSKAPR020</t>
-  </si>
-  <si>
     <t>## WHOLE GENOME ANALYSIS BASED ON COVERAGE##</t>
   </si>
   <si>
@@ -1864,13 +1861,7 @@
     <t xml:space="preserve">1508:22 Orderform </t>
   </si>
   <si>
-    <t>Added Delivery</t>
-  </si>
-  <si>
     <t>WGTLIFC030</t>
-  </si>
-  <si>
-    <t>Removed application tags: WGSPCFC060, WGSPCFC090</t>
   </si>
   <si>
     <t>Added application tags: WGSPCFS120, WGSPCFR800, WGSPCFR400, WGSLIFS120, WGSLIFR800, WGSLIFR400, WGTLIFC030</t>
@@ -1896,9 +1887,6 @@
   </si>
   <si>
     <t>Added Volume (uL)</t>
-  </si>
-  <si>
-    <t>fastq</t>
   </si>
   <si>
     <t>UDF/Data Delivery</t>
@@ -1947,22 +1935,13 @@
     <t>Balsamic</t>
   </si>
   <si>
-    <t>Balsamic QC</t>
-  </si>
-  <si>
     <t>No analysis</t>
   </si>
   <si>
     <t>Analysis</t>
   </si>
   <si>
-    <t>Analysis BAM</t>
-  </si>
-  <si>
     <t>Scout</t>
-  </si>
-  <si>
-    <t>Added options for Data Analysis: Balsamic QC, No analysis</t>
   </si>
   <si>
     <r>
@@ -1994,223 +1973,6 @@
       </rPr>
       <t xml:space="preserve">States the application of the order. Options available in drop down list. For more information about the different application tags see: https://clinical.scilifelab.se/applications
 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Data Delivery: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Options for how the data should be delivered. Options available in drop down list. Only one option can be chosen. If more than one option is wanted, please contact Clinical Genomics.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Fastq</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = fastq-files (raw data). Option only available for the option "No analysis" in Data Analysis.  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Analysis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = files generated by chosen Data Analysis option. File package differ between pipelines. Option available for all options in Data Analysis except "No Analysis".
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Analysis BAM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = files generated by analysis pipeline Balsamic and will be delivered to delivery server Caesar, including bam-files. Option only available for Balsamic (Balsamic has 2 different analysis-packages, this includes bam-files).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Scout</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = Cases will be uploaded to our customer-facing variant browser Scout. Access for every new user is needed. Option available for MIP DNA and Balsamic.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Data Analysis:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Options for different types of analyses/pipelines of human samples. Options available in drop down list. Connect samples by using Case ID. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>MIP DNA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = Mutation Identification Pipeline, analysis of germline variants (used also for some hereditary cancers) for DNA, 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Balsamic</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = Cancer pipeline, analysis of somatic variants. Only-tumour analysis OR tumour/normal with only 1 tumour per normal allowed per case.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Balsamic QC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Cancer pipeline for only QC analysis with MultiQC report and trimmed fastq-files. Only-tumour analysis OR tumour/normal with only 1 tumour per normal allowed per case.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">MIP RNA </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">= Mutation Identification Pipeline, analysis of RNA. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>No analysis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = No analysis will be done, only sequencing and delivery of raw data (fastq-files).</t>
     </r>
   </si>
   <si>
@@ -2419,10 +2181,233 @@
     </r>
   </si>
   <si>
-    <t>s1</t>
+    <t>Fastq</t>
   </si>
   <si>
-    <t>c1</t>
+    <t>Fastq QC</t>
+  </si>
+  <si>
+    <r>
+      <t>Data Analysis:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Options for different types of analyses/pipelines of human samples. Options available in drop down list. Connect samples by using Case ID. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>MIP DNA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = Mutation Identification Pipeline, analysis of germline variants (used also for some hereditary cancers) for DNA, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Balsamic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = Cancer pipeline, analysis of somatic variants. Only-tumour analysis OR tumour/normal with only 1 tumour per normal allowed per case.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">MIP RNA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">= Mutation Identification Pipeline, analysis of RNA. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>No analysis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = No analysis will be done, only sequencing and delivery of raw data (fastq-files).</t>
+    </r>
+  </si>
+  <si>
+    <t>Added option "No Analysis" for Data Analysis</t>
+  </si>
+  <si>
+    <t>Added Delivery with options</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data Delivery: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Options for how the data should be delivered. Options available in drop down list. Only one option can be chosen. If more than one option is wanted, please contact Clinical Genomics.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Fastq</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = fastq-files (raw data). Option only available for the option "No analysis" in Data Analysis.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Fastq QC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = fastq-files (raw data) with QC analysis including MultiQC report and trimmed Fastq-files. Only available for option Balsamic in Data Analysis.    
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Analysis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = files generated by chosen Data Analysis option. File package differ between pipelines. Option available for all options in Data Analysis except "No Analysis".
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Analysis + BAM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = files generated by analysis pipeline Balsamic and will be delivered to delivery server Caesar, including bam-files. Option only available for option Balsamic in Data Analysis (Balsamic has 2 different analysis-packages, this includes bam-files).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Scout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = Cases will be uploaded to our customer-facing variant browser Scout. Access for every new user is needed. Option available for MIP DNA and Balsamic.</t>
+    </r>
+  </si>
+  <si>
+    <t>Analysis + BAM</t>
+  </si>
+  <si>
+    <t>Removed application tags: WGSPCFC060, WGSPCFC090, WGSKAPR020</t>
+  </si>
+  <si>
+    <t>s1</t>
   </si>
   <si>
     <t>s2</t>
@@ -2431,214 +2416,7 @@
     <t>s3</t>
   </si>
   <si>
-    <t>s4</t>
-  </si>
-  <si>
-    <t>s5</t>
-  </si>
-  <si>
-    <t>s6</t>
-  </si>
-  <si>
-    <t>s7</t>
-  </si>
-  <si>
-    <t>s8</t>
-  </si>
-  <si>
-    <t>s9</t>
-  </si>
-  <si>
-    <t>s10</t>
-  </si>
-  <si>
-    <t>s11</t>
-  </si>
-  <si>
-    <t>s12</t>
-  </si>
-  <si>
-    <t>s13</t>
-  </si>
-  <si>
-    <t>s14</t>
-  </si>
-  <si>
-    <t>s15</t>
-  </si>
-  <si>
-    <t>s16</t>
-  </si>
-  <si>
-    <t>s17</t>
-  </si>
-  <si>
-    <t>s18</t>
-  </si>
-  <si>
-    <t>s19</t>
-  </si>
-  <si>
-    <t>s20</t>
-  </si>
-  <si>
-    <t>s21</t>
-  </si>
-  <si>
-    <t>s22</t>
-  </si>
-  <si>
-    <t>s23</t>
-  </si>
-  <si>
-    <t>s24</t>
-  </si>
-  <si>
-    <t>s25</t>
-  </si>
-  <si>
-    <t>s26</t>
-  </si>
-  <si>
-    <t>s27</t>
-  </si>
-  <si>
-    <t>s28</t>
-  </si>
-  <si>
-    <t>s29</t>
-  </si>
-  <si>
-    <t>s30</t>
-  </si>
-  <si>
-    <t>s31</t>
-  </si>
-  <si>
-    <t>s32</t>
-  </si>
-  <si>
-    <t>s33</t>
-  </si>
-  <si>
-    <t>s34</t>
-  </si>
-  <si>
-    <t>s35</t>
-  </si>
-  <si>
-    <t>s36</t>
-  </si>
-  <si>
-    <t>s37</t>
-  </si>
-  <si>
-    <t>s38</t>
-  </si>
-  <si>
-    <t>c2</t>
-  </si>
-  <si>
-    <t>c3</t>
-  </si>
-  <si>
-    <t>c4</t>
-  </si>
-  <si>
-    <t>c5</t>
-  </si>
-  <si>
-    <t>c6</t>
-  </si>
-  <si>
-    <t>c7</t>
-  </si>
-  <si>
-    <t>c8</t>
-  </si>
-  <si>
-    <t>c9</t>
-  </si>
-  <si>
-    <t>c10</t>
-  </si>
-  <si>
-    <t>c11</t>
-  </si>
-  <si>
-    <t>c12</t>
-  </si>
-  <si>
-    <t>c13</t>
-  </si>
-  <si>
-    <t>c14</t>
-  </si>
-  <si>
-    <t>c15</t>
-  </si>
-  <si>
-    <t>c16</t>
-  </si>
-  <si>
-    <t>c17</t>
-  </si>
-  <si>
-    <t>c18</t>
-  </si>
-  <si>
-    <t>c19</t>
-  </si>
-  <si>
-    <t>c20</t>
-  </si>
-  <si>
-    <t>c21</t>
-  </si>
-  <si>
-    <t>c22</t>
-  </si>
-  <si>
-    <t>c23</t>
-  </si>
-  <si>
-    <t>c24</t>
-  </si>
-  <si>
-    <t>c25</t>
-  </si>
-  <si>
-    <t>c26</t>
-  </si>
-  <si>
-    <t>c27</t>
-  </si>
-  <si>
-    <t>c28</t>
-  </si>
-  <si>
-    <t>c29</t>
-  </si>
-  <si>
-    <t>c30</t>
-  </si>
-  <si>
-    <t>c31</t>
-  </si>
-  <si>
-    <t>c32</t>
-  </si>
-  <si>
-    <t>c33</t>
-  </si>
-  <si>
-    <t>c34</t>
-  </si>
-  <si>
-    <t>c35</t>
-  </si>
-  <si>
-    <t>c36</t>
+    <t>c1</t>
   </si>
   <si>
     <t>plate1</t>
@@ -2647,10 +2425,223 @@
     <t>GMCKsolid</t>
   </si>
   <si>
-    <t>other Elution buffer</t>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>s4</t>
+  </si>
+  <si>
+    <t>s5</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>s6</t>
+  </si>
+  <si>
+    <t>c4</t>
+  </si>
+  <si>
+    <t>s7</t>
+  </si>
+  <si>
+    <t>WGSKAPR020</t>
+  </si>
+  <si>
+    <t>c5</t>
+  </si>
+  <si>
+    <t>s8</t>
+  </si>
+  <si>
+    <t>c6</t>
+  </si>
+  <si>
+    <t>s9</t>
+  </si>
+  <si>
+    <t>c7</t>
+  </si>
+  <si>
+    <t>s10</t>
+  </si>
+  <si>
+    <t>c8</t>
+  </si>
+  <si>
+    <t>s11</t>
+  </si>
+  <si>
+    <t>c9</t>
+  </si>
+  <si>
+    <t>s12</t>
+  </si>
+  <si>
+    <t>c10</t>
+  </si>
+  <si>
+    <t>s13</t>
+  </si>
+  <si>
+    <t>c11</t>
+  </si>
+  <si>
+    <t>s14</t>
+  </si>
+  <si>
+    <t>c12</t>
+  </si>
+  <si>
+    <t>s15</t>
+  </si>
+  <si>
+    <t>c13</t>
+  </si>
+  <si>
+    <t>s16</t>
+  </si>
+  <si>
+    <t>c14</t>
+  </si>
+  <si>
+    <t>s17</t>
+  </si>
+  <si>
+    <t>c15</t>
+  </si>
+  <si>
+    <t>s18</t>
+  </si>
+  <si>
+    <t>c16</t>
+  </si>
+  <si>
+    <t>s19</t>
+  </si>
+  <si>
+    <t>c17</t>
+  </si>
+  <si>
+    <t>s20</t>
+  </si>
+  <si>
+    <t>c18</t>
+  </si>
+  <si>
+    <t>s21</t>
+  </si>
+  <si>
+    <t>c19</t>
+  </si>
+  <si>
+    <t>s22</t>
+  </si>
+  <si>
+    <t>c20</t>
+  </si>
+  <si>
+    <t>s23</t>
+  </si>
+  <si>
+    <t>c21</t>
+  </si>
+  <si>
+    <t>s24</t>
+  </si>
+  <si>
+    <t>c22</t>
+  </si>
+  <si>
+    <t>s25</t>
+  </si>
+  <si>
+    <t>c23</t>
+  </si>
+  <si>
+    <t>s26</t>
+  </si>
+  <si>
+    <t>c24</t>
+  </si>
+  <si>
+    <t>s27</t>
+  </si>
+  <si>
+    <t>c25</t>
+  </si>
+  <si>
+    <t>s28</t>
+  </si>
+  <si>
+    <t>c26</t>
+  </si>
+  <si>
+    <t>s29</t>
+  </si>
+  <si>
+    <t>c27</t>
+  </si>
+  <si>
+    <t>s30</t>
+  </si>
+  <si>
+    <t>c28</t>
+  </si>
+  <si>
+    <t>s31</t>
+  </si>
+  <si>
+    <t>c29</t>
+  </si>
+  <si>
+    <t>s32</t>
+  </si>
+  <si>
+    <t>c30</t>
+  </si>
+  <si>
+    <t>s33</t>
+  </si>
+  <si>
+    <t>c31</t>
+  </si>
+  <si>
+    <t>s34</t>
+  </si>
+  <si>
+    <t>c32</t>
+  </si>
+  <si>
+    <t>s35</t>
+  </si>
+  <si>
+    <t>c33</t>
+  </si>
+  <si>
+    <t>s36</t>
+  </si>
+  <si>
+    <t>c34</t>
+  </si>
+  <si>
+    <t>s37</t>
+  </si>
+  <si>
+    <t>c35</t>
+  </si>
+  <si>
+    <t>s38</t>
+  </si>
+  <si>
+    <t>c36</t>
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>other Elution buffer</t>
   </si>
 </sst>
 </file>
@@ -2661,7 +2652,7 @@
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="53">
+  <fonts count="52">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2997,13 +2988,6 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3326,7 +3310,7 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
@@ -3753,34 +3737,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3816,6 +3772,26 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="24">
@@ -4347,7 +4323,7 @@
   <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4364,7 +4340,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="113" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D1" s="114"/>
       <c r="E1" s="115"/>
@@ -4422,42 +4398,42 @@
     </row>
     <row r="16" spans="1:5" ht="14" customHeight="1">
       <c r="A16" s="116" t="s">
-        <v>530</v>
+        <v>558</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14" customHeight="1">
       <c r="A17" s="116" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14" customHeight="1">
       <c r="A18" s="124" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="116" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="28">
       <c r="A20" s="124" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="14">
       <c r="A21" s="124" t="s">
-        <v>532</v>
+        <v>561</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="116" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="116" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="16">
@@ -4471,34 +4447,34 @@
       </c>
     </row>
     <row r="26" spans="1:1" ht="8" customHeight="1"/>
-    <row r="27" spans="1:1" ht="41" customHeight="1">
+    <row r="27" spans="1:1" ht="37" customHeight="1">
       <c r="A27" s="127" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="24" customHeight="1">
+    <row r="28" spans="1:1" ht="26" customHeight="1">
       <c r="A28" s="128" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="135" customHeight="1">
+    <row r="29" spans="1:1" ht="105" customHeight="1">
       <c r="A29" s="128" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="140" customHeight="1">
+    <row r="30" spans="1:1" ht="165" customHeight="1">
       <c r="A30" s="128" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="46" customHeight="1">
       <c r="A31" s="128" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="57" customHeight="1">
       <c r="A32" s="128" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="26" customHeight="1">
@@ -4518,7 +4494,7 @@
     </row>
     <row r="36" spans="1:5" ht="25" customHeight="1">
       <c r="A36" s="127" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="57" customHeight="1">
@@ -4530,7 +4506,7 @@
     </row>
     <row r="38" spans="1:5" ht="16" customHeight="1">
       <c r="A38" s="127" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C38" s="124"/>
       <c r="E38" s="124"/>
@@ -4551,14 +4527,14 @@
     </row>
     <row r="42" spans="1:5" ht="28" customHeight="1">
       <c r="A42" s="127" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="C42" s="124"/>
       <c r="E42" s="124"/>
     </row>
     <row r="43" spans="1:5" ht="26" customHeight="1">
       <c r="A43" s="127" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="C43" s="124"/>
       <c r="E43" s="124"/>
@@ -4572,7 +4548,7 @@
     <row r="45" spans="1:5" ht="6" customHeight="1"/>
     <row r="46" spans="1:5" ht="38" customHeight="1">
       <c r="A46" s="127" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="26" customHeight="1">
@@ -4603,7 +4579,7 @@
     </row>
     <row r="53" spans="1:1" ht="33" customHeight="1">
       <c r="A53" s="127" t="s">
-        <v>560</v>
+        <v>551</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="20" customHeight="1">
@@ -4626,7 +4602,7 @@
     </row>
     <row r="58" spans="1:1" ht="44" customHeight="1">
       <c r="A58" s="130" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="20" customHeight="1">
@@ -4658,7 +4634,7 @@
     <row r="65" spans="1:1" ht="7" customHeight="1"/>
     <row r="66" spans="1:1" ht="15" customHeight="1">
       <c r="A66" s="127" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="31" customHeight="1">
@@ -4711,7 +4687,6 @@
       <c r="A85" s="124"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ZlBvTOjGXJp939cmWVpSY0Q40Undp1saY4b8X89aAA43ujjQOb10T5u2cR58ydn1AQSm3hEa/9cfVMI7gTsUYQ==" saltValue="OO3fdrt6el02uVo2rNdGOg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
@@ -4733,8 +4708,8 @@
   </sheetPr>
   <dimension ref="A1:AMM395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:H52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1"/>
@@ -11023,38 +10998,38 @@
       <c r="AJ8" s="39"/>
     </row>
     <row r="9" spans="1:1026" s="45" customFormat="1" ht="22" customHeight="1" outlineLevel="1">
-      <c r="A9" s="178" t="s">
+      <c r="A9" s="169" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="179"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
-      <c r="G9" s="179"/>
-      <c r="H9" s="179"/>
-      <c r="I9" s="179"/>
-      <c r="J9" s="179"/>
-      <c r="K9" s="179"/>
-      <c r="L9" s="179"/>
-      <c r="M9" s="180"/>
+      <c r="B9" s="170"/>
+      <c r="C9" s="170"/>
+      <c r="D9" s="170"/>
+      <c r="E9" s="170"/>
+      <c r="F9" s="170"/>
+      <c r="G9" s="170"/>
+      <c r="H9" s="170"/>
+      <c r="I9" s="170"/>
+      <c r="J9" s="170"/>
+      <c r="K9" s="170"/>
+      <c r="L9" s="170"/>
+      <c r="M9" s="171"/>
       <c r="N9" s="41"/>
-      <c r="O9" s="182" t="s">
+      <c r="O9" s="173" t="s">
         <v>22</v>
       </c>
-      <c r="P9" s="182"/>
+      <c r="P9" s="173"/>
       <c r="Q9" s="133"/>
-      <c r="R9" s="184" t="s">
+      <c r="R9" s="175" t="s">
         <v>23</v>
       </c>
-      <c r="S9" s="185"/>
-      <c r="T9" s="185"/>
-      <c r="U9" s="186"/>
+      <c r="S9" s="176"/>
+      <c r="T9" s="176"/>
+      <c r="U9" s="177"/>
       <c r="V9" s="42"/>
-      <c r="W9" s="183" t="s">
+      <c r="W9" s="174" t="s">
         <v>517</v>
       </c>
-      <c r="X9" s="183"/>
+      <c r="X9" s="174"/>
       <c r="Y9" s="42"/>
       <c r="Z9" s="43" t="s">
         <v>24</v>
@@ -11064,17 +11039,17 @@
         <v>25</v>
       </c>
       <c r="AC9" s="44"/>
-      <c r="AD9" s="181" t="s">
+      <c r="AD9" s="172" t="s">
         <v>26</v>
       </c>
-      <c r="AE9" s="181"/>
-      <c r="AF9" s="181"/>
+      <c r="AE9" s="172"/>
+      <c r="AF9" s="172"/>
       <c r="AG9" s="42"/>
-      <c r="AH9" s="175" t="s">
+      <c r="AH9" s="166" t="s">
         <v>15</v>
       </c>
-      <c r="AI9" s="176"/>
-      <c r="AJ9" s="177"/>
+      <c r="AI9" s="167"/>
+      <c r="AJ9" s="168"/>
     </row>
     <row r="10" spans="1:1026" ht="13" hidden="1" customHeight="1">
       <c r="A10" s="46" t="s">
@@ -12117,7 +12092,7 @@
         <v>30</v>
       </c>
       <c r="D11" s="161" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="E11" s="49" t="s">
         <v>31</v>
@@ -12141,7 +12116,7 @@
         <v>37</v>
       </c>
       <c r="L11" s="53" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="M11" s="49" t="s">
         <v>38</v>
@@ -12253,7 +12228,7 @@
         <v>58</v>
       </c>
       <c r="D13" s="70" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E13" s="70" t="s">
         <v>59</v>
@@ -12277,7 +12252,7 @@
         <v>65</v>
       </c>
       <c r="L13" s="69" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="M13" s="70" t="s">
         <v>66</v>
@@ -12380,22 +12355,22 @@
     </row>
     <row r="15" spans="1:1026" ht="25" customHeight="1">
       <c r="A15" s="82" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B15" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C15" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D15" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E15" s="84" t="s">
         <v>211</v>
       </c>
       <c r="F15" s="82" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="G15" s="85" t="s">
         <v>89</v>
@@ -12403,7 +12378,7 @@
       <c r="H15" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="169" t="s">
+      <c r="I15" s="178" t="s">
         <v>162</v>
       </c>
       <c r="J15" s="104" t="s">
@@ -12420,13 +12395,13 @@
       </c>
       <c r="N15" s="87"/>
       <c r="O15" s="88" t="s">
-        <v>637</v>
+        <v>566</v>
       </c>
       <c r="P15" s="107" t="s">
         <v>96</v>
       </c>
       <c r="Q15" s="54"/>
-      <c r="R15" s="169"/>
+      <c r="R15" s="110"/>
       <c r="S15" s="138"/>
       <c r="T15" s="82"/>
       <c r="U15" s="89"/>
@@ -12434,11 +12409,11 @@
       <c r="W15" s="82"/>
       <c r="X15" s="108"/>
       <c r="Y15" s="90"/>
-      <c r="Z15" s="109" t="s">
-        <v>638</v>
+      <c r="Z15" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA15" s="92"/>
-      <c r="AB15" s="169" t="s">
+      <c r="AB15" s="178" t="s">
         <v>122</v>
       </c>
       <c r="AC15" s="92"/>
@@ -12453,13 +12428,13 @@
       </c>
       <c r="AG15" s="61"/>
       <c r="AH15" s="88" t="s">
+        <v>639</v>
+      </c>
+      <c r="AI15" s="182">
+        <v>5</v>
+      </c>
+      <c r="AJ15" s="183" t="s">
         <v>640</v>
-      </c>
-      <c r="AI15" s="110">
-        <v>5</v>
-      </c>
-      <c r="AJ15" s="172" t="s">
-        <v>639</v>
       </c>
       <c r="AK15"/>
       <c r="AL15"/>
@@ -13454,22 +13429,22 @@
     </row>
     <row r="16" spans="1:1026" ht="25" customHeight="1">
       <c r="A16" s="82" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B16" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C16" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D16" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E16" s="84" t="s">
         <v>130</v>
       </c>
       <c r="F16" s="82" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="G16" s="85" t="s">
         <v>101</v>
@@ -13477,7 +13452,7 @@
       <c r="H16" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="I16" s="170" t="s">
+      <c r="I16" s="179" t="s">
         <v>104</v>
       </c>
       <c r="J16" s="104" t="s">
@@ -13496,7 +13471,7 @@
       <c r="O16" s="88"/>
       <c r="P16" s="107"/>
       <c r="Q16" s="54"/>
-      <c r="R16" s="169"/>
+      <c r="R16" s="110"/>
       <c r="S16" s="138"/>
       <c r="T16" s="93"/>
       <c r="U16" s="94"/>
@@ -13504,7 +13479,7 @@
       <c r="W16" s="82"/>
       <c r="X16" s="108"/>
       <c r="Y16" s="90"/>
-      <c r="Z16" s="109"/>
+      <c r="Z16" s="181"/>
       <c r="AA16" s="92"/>
       <c r="AB16" s="91"/>
       <c r="AC16" s="92"/>
@@ -14508,22 +14483,22 @@
     </row>
     <row r="17" spans="1:1026" ht="25" customHeight="1">
       <c r="A17" s="82" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B17" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D17" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E17" s="84" t="s">
         <v>135</v>
       </c>
       <c r="F17" s="82" t="s">
-        <v>602</v>
+        <v>568</v>
       </c>
       <c r="G17" s="85" t="s">
         <v>112</v>
@@ -14531,7 +14506,7 @@
       <c r="H17" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I17" s="169" t="s">
+      <c r="I17" s="178" t="s">
         <v>114</v>
       </c>
       <c r="J17" s="104" t="s">
@@ -14550,7 +14525,7 @@
       <c r="O17" s="88"/>
       <c r="P17" s="107"/>
       <c r="Q17" s="54"/>
-      <c r="R17" s="169"/>
+      <c r="R17" s="110"/>
       <c r="S17" s="138"/>
       <c r="T17" s="93"/>
       <c r="U17" s="94"/>
@@ -14558,7 +14533,7 @@
       <c r="W17" s="89"/>
       <c r="X17" s="108"/>
       <c r="Y17" s="90"/>
-      <c r="Z17" s="109"/>
+      <c r="Z17" s="181"/>
       <c r="AA17" s="92"/>
       <c r="AB17" s="91"/>
       <c r="AC17" s="92"/>
@@ -15562,22 +15537,22 @@
     </row>
     <row r="18" spans="1:1026" ht="25" customHeight="1">
       <c r="A18" s="82" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="B18" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C18" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D18" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E18" s="84" t="s">
         <v>111</v>
       </c>
       <c r="F18" s="82" t="s">
-        <v>602</v>
+        <v>568</v>
       </c>
       <c r="G18" s="85" t="s">
         <v>112</v>
@@ -15585,7 +15560,7 @@
       <c r="H18" s="86" t="s">
         <v>103</v>
       </c>
-      <c r="I18" s="170" t="s">
+      <c r="I18" s="179" t="s">
         <v>120</v>
       </c>
       <c r="J18" s="104" t="s">
@@ -15604,7 +15579,7 @@
       <c r="O18" s="88"/>
       <c r="P18" s="107"/>
       <c r="Q18" s="54"/>
-      <c r="R18" s="169"/>
+      <c r="R18" s="110"/>
       <c r="S18" s="138"/>
       <c r="T18" s="93"/>
       <c r="U18" s="94"/>
@@ -15612,7 +15587,7 @@
       <c r="W18" s="95"/>
       <c r="X18" s="108"/>
       <c r="Y18" s="90"/>
-      <c r="Z18" s="109"/>
+      <c r="Z18" s="181"/>
       <c r="AA18" s="92"/>
       <c r="AB18" s="91"/>
       <c r="AC18" s="92"/>
@@ -16616,22 +16591,22 @@
     </row>
     <row r="19" spans="1:1026" ht="25" customHeight="1">
       <c r="A19" s="82" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B19" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C19" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D19" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E19" s="84" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F19" s="82" t="s">
-        <v>603</v>
+        <v>571</v>
       </c>
       <c r="G19" s="85" t="s">
         <v>112</v>
@@ -16639,7 +16614,7 @@
       <c r="H19" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I19" s="169" t="s">
+      <c r="I19" s="178" t="s">
         <v>126</v>
       </c>
       <c r="J19" s="104" t="s">
@@ -16658,7 +16633,7 @@
       <c r="O19" s="88"/>
       <c r="P19" s="107"/>
       <c r="Q19" s="54"/>
-      <c r="R19" s="169"/>
+      <c r="R19" s="110"/>
       <c r="S19" s="138"/>
       <c r="T19" s="93"/>
       <c r="U19" s="94"/>
@@ -16666,7 +16641,7 @@
       <c r="W19" s="95"/>
       <c r="X19" s="108"/>
       <c r="Y19" s="90"/>
-      <c r="Z19" s="109"/>
+      <c r="Z19" s="181"/>
       <c r="AA19" s="92"/>
       <c r="AB19" s="91"/>
       <c r="AC19" s="92"/>
@@ -17670,22 +17645,22 @@
     </row>
     <row r="20" spans="1:1026" ht="25" customHeight="1">
       <c r="A20" s="82" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="B20" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C20" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D20" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E20" s="84" t="s">
         <v>140</v>
       </c>
       <c r="F20" s="82" t="s">
-        <v>604</v>
+        <v>573</v>
       </c>
       <c r="G20" s="85" t="s">
         <v>112</v>
@@ -17693,7 +17668,7 @@
       <c r="H20" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I20" s="171" t="s">
+      <c r="I20" s="180" t="s">
         <v>126</v>
       </c>
       <c r="J20" s="104" t="s">
@@ -17712,7 +17687,7 @@
       <c r="O20" s="88"/>
       <c r="P20" s="107"/>
       <c r="Q20" s="54"/>
-      <c r="R20" s="169"/>
+      <c r="R20" s="110"/>
       <c r="S20" s="138"/>
       <c r="T20" s="93"/>
       <c r="U20" s="94"/>
@@ -17720,7 +17695,7 @@
       <c r="W20" s="95"/>
       <c r="X20" s="108"/>
       <c r="Y20" s="90"/>
-      <c r="Z20" s="109"/>
+      <c r="Z20" s="181"/>
       <c r="AA20" s="92"/>
       <c r="AB20" s="91"/>
       <c r="AC20" s="92"/>
@@ -18724,22 +18699,22 @@
     </row>
     <row r="21" spans="1:1026" ht="25" customHeight="1">
       <c r="A21" s="82" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="B21" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C21" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D21" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E21" s="84" t="s">
-        <v>518</v>
+        <v>575</v>
       </c>
       <c r="F21" s="82" t="s">
-        <v>605</v>
+        <v>576</v>
       </c>
       <c r="G21" s="85" t="s">
         <v>112</v>
@@ -18747,7 +18722,7 @@
       <c r="H21" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I21" s="171" t="s">
+      <c r="I21" s="180" t="s">
         <v>137</v>
       </c>
       <c r="J21" s="104" t="s">
@@ -18766,7 +18741,7 @@
       <c r="O21" s="88"/>
       <c r="P21" s="107"/>
       <c r="Q21" s="54"/>
-      <c r="R21" s="169"/>
+      <c r="R21" s="110"/>
       <c r="S21" s="138"/>
       <c r="T21" s="93"/>
       <c r="U21" s="94"/>
@@ -18774,7 +18749,7 @@
       <c r="W21" s="95"/>
       <c r="X21" s="108"/>
       <c r="Y21" s="90"/>
-      <c r="Z21" s="109"/>
+      <c r="Z21" s="181"/>
       <c r="AA21" s="92"/>
       <c r="AB21" s="91"/>
       <c r="AC21" s="92"/>
@@ -19778,22 +19753,22 @@
     </row>
     <row r="22" spans="1:1026" ht="25" customHeight="1">
       <c r="A22" s="82" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="B22" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C22" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D22" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E22" s="84" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F22" s="82" t="s">
-        <v>606</v>
+        <v>578</v>
       </c>
       <c r="G22" s="85" t="s">
         <v>112</v>
@@ -19801,7 +19776,7 @@
       <c r="H22" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I22" s="169" t="s">
+      <c r="I22" s="178" t="s">
         <v>142</v>
       </c>
       <c r="J22" s="104" t="s">
@@ -19820,7 +19795,7 @@
       <c r="O22" s="88"/>
       <c r="P22" s="107"/>
       <c r="Q22" s="54"/>
-      <c r="R22" s="169"/>
+      <c r="R22" s="110"/>
       <c r="S22" s="138"/>
       <c r="T22" s="93"/>
       <c r="U22" s="94"/>
@@ -19828,7 +19803,7 @@
       <c r="W22" s="95"/>
       <c r="X22" s="108"/>
       <c r="Y22" s="90"/>
-      <c r="Z22" s="109"/>
+      <c r="Z22" s="181"/>
       <c r="AA22" s="92"/>
       <c r="AB22" s="91"/>
       <c r="AC22" s="92"/>
@@ -20832,22 +20807,22 @@
     </row>
     <row r="23" spans="1:1026" ht="25" customHeight="1">
       <c r="A23" s="82" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="B23" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C23" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D23" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E23" s="84" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F23" s="82" t="s">
-        <v>607</v>
+        <v>580</v>
       </c>
       <c r="G23" s="85" t="s">
         <v>112</v>
@@ -20855,7 +20830,7 @@
       <c r="H23" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I23" s="169" t="s">
+      <c r="I23" s="178" t="s">
         <v>147</v>
       </c>
       <c r="J23" s="104" t="s">
@@ -20874,7 +20849,7 @@
       <c r="O23" s="88"/>
       <c r="P23" s="107"/>
       <c r="Q23" s="54"/>
-      <c r="R23" s="169"/>
+      <c r="R23" s="110"/>
       <c r="S23" s="138"/>
       <c r="T23" s="93"/>
       <c r="U23" s="94"/>
@@ -20882,7 +20857,7 @@
       <c r="W23" s="95"/>
       <c r="X23" s="108"/>
       <c r="Y23" s="90"/>
-      <c r="Z23" s="109"/>
+      <c r="Z23" s="181"/>
       <c r="AA23" s="92"/>
       <c r="AB23" s="91"/>
       <c r="AC23" s="92"/>
@@ -21886,22 +21861,22 @@
     </row>
     <row r="24" spans="1:1026" ht="25" customHeight="1">
       <c r="A24" s="82" t="s">
-        <v>573</v>
+        <v>581</v>
       </c>
       <c r="B24" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C24" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D24" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E24" s="84" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F24" s="82" t="s">
-        <v>608</v>
+        <v>582</v>
       </c>
       <c r="G24" s="85" t="s">
         <v>112</v>
@@ -21909,7 +21884,7 @@
       <c r="H24" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I24" s="169" t="s">
+      <c r="I24" s="178" t="s">
         <v>152</v>
       </c>
       <c r="J24" s="104" t="s">
@@ -21928,7 +21903,7 @@
       <c r="O24" s="88"/>
       <c r="P24" s="107"/>
       <c r="Q24" s="54"/>
-      <c r="R24" s="169"/>
+      <c r="R24" s="110"/>
       <c r="S24" s="138"/>
       <c r="T24" s="93"/>
       <c r="U24" s="94"/>
@@ -21936,7 +21911,7 @@
       <c r="W24" s="95"/>
       <c r="X24" s="108"/>
       <c r="Y24" s="90"/>
-      <c r="Z24" s="109"/>
+      <c r="Z24" s="181"/>
       <c r="AA24" s="92"/>
       <c r="AB24" s="91"/>
       <c r="AC24" s="92"/>
@@ -22940,22 +22915,22 @@
     </row>
     <row r="25" spans="1:1026" ht="25" customHeight="1">
       <c r="A25" s="82" t="s">
-        <v>574</v>
+        <v>583</v>
       </c>
       <c r="B25" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C25" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D25" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E25" s="84" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F25" s="82" t="s">
-        <v>609</v>
+        <v>584</v>
       </c>
       <c r="G25" s="85" t="s">
         <v>112</v>
@@ -22963,7 +22938,7 @@
       <c r="H25" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I25" s="169" t="s">
+      <c r="I25" s="178" t="s">
         <v>157</v>
       </c>
       <c r="J25" s="104" t="s">
@@ -22982,7 +22957,7 @@
       <c r="O25" s="88"/>
       <c r="P25" s="107"/>
       <c r="Q25" s="54"/>
-      <c r="R25" s="169"/>
+      <c r="R25" s="110"/>
       <c r="S25" s="138"/>
       <c r="T25" s="93"/>
       <c r="U25" s="94"/>
@@ -22990,7 +22965,7 @@
       <c r="W25" s="95"/>
       <c r="X25" s="108"/>
       <c r="Y25" s="90"/>
-      <c r="Z25" s="109"/>
+      <c r="Z25" s="181"/>
       <c r="AA25" s="92"/>
       <c r="AB25" s="91"/>
       <c r="AC25" s="92"/>
@@ -23994,22 +23969,22 @@
     </row>
     <row r="26" spans="1:1026" ht="25" customHeight="1">
       <c r="A26" s="82" t="s">
-        <v>575</v>
+        <v>585</v>
       </c>
       <c r="B26" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C26" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D26" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E26" s="84" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F26" s="82" t="s">
-        <v>610</v>
+        <v>586</v>
       </c>
       <c r="G26" s="85" t="s">
         <v>112</v>
@@ -24017,7 +23992,7 @@
       <c r="H26" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I26" s="169" t="s">
+      <c r="I26" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J26" s="104" t="s">
@@ -24036,7 +24011,7 @@
       <c r="O26" s="88"/>
       <c r="P26" s="107"/>
       <c r="Q26" s="54"/>
-      <c r="R26" s="169"/>
+      <c r="R26" s="110"/>
       <c r="S26" s="138"/>
       <c r="T26" s="93"/>
       <c r="U26" s="94"/>
@@ -24044,7 +24019,7 @@
       <c r="W26" s="95"/>
       <c r="X26" s="108"/>
       <c r="Y26" s="90"/>
-      <c r="Z26" s="109"/>
+      <c r="Z26" s="181"/>
       <c r="AA26" s="92"/>
       <c r="AB26" s="91"/>
       <c r="AC26" s="92"/>
@@ -25048,22 +25023,22 @@
     </row>
     <row r="27" spans="1:1026" s="96" customFormat="1" ht="25" customHeight="1">
       <c r="A27" s="82" t="s">
-        <v>576</v>
+        <v>587</v>
       </c>
       <c r="B27" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C27" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D27" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E27" s="84" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F27" s="82" t="s">
-        <v>611</v>
+        <v>588</v>
       </c>
       <c r="G27" s="85" t="s">
         <v>112</v>
@@ -25071,7 +25046,7 @@
       <c r="H27" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I27" s="169" t="s">
+      <c r="I27" s="178" t="s">
         <v>167</v>
       </c>
       <c r="J27" s="104" t="s">
@@ -25090,7 +25065,7 @@
       <c r="O27" s="88"/>
       <c r="P27" s="107"/>
       <c r="Q27" s="54"/>
-      <c r="R27" s="169"/>
+      <c r="R27" s="110"/>
       <c r="S27" s="138"/>
       <c r="T27" s="93"/>
       <c r="U27" s="94"/>
@@ -25098,7 +25073,7 @@
       <c r="W27" s="95"/>
       <c r="X27" s="108"/>
       <c r="Y27" s="90"/>
-      <c r="Z27" s="109"/>
+      <c r="Z27" s="181"/>
       <c r="AA27" s="92"/>
       <c r="AB27" s="91"/>
       <c r="AC27" s="92"/>
@@ -25112,22 +25087,22 @@
     </row>
     <row r="28" spans="1:1026" ht="25" customHeight="1">
       <c r="A28" s="82" t="s">
-        <v>577</v>
+        <v>589</v>
       </c>
       <c r="B28" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C28" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D28" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E28" s="84" t="s">
         <v>150</v>
       </c>
       <c r="F28" s="82" t="s">
-        <v>612</v>
+        <v>590</v>
       </c>
       <c r="G28" s="85" t="s">
         <v>112</v>
@@ -25135,7 +25110,7 @@
       <c r="H28" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I28" s="169" t="s">
+      <c r="I28" s="178" t="s">
         <v>132</v>
       </c>
       <c r="J28" s="104" t="s">
@@ -25154,7 +25129,7 @@
       <c r="O28" s="88"/>
       <c r="P28" s="107"/>
       <c r="Q28" s="54"/>
-      <c r="R28" s="169"/>
+      <c r="R28" s="110"/>
       <c r="S28" s="138"/>
       <c r="T28" s="93"/>
       <c r="U28" s="94"/>
@@ -25162,9 +25137,9 @@
       <c r="W28" s="95"/>
       <c r="X28" s="108"/>
       <c r="Y28" s="90"/>
-      <c r="Z28" s="109"/>
+      <c r="Z28" s="181"/>
       <c r="AA28" s="92"/>
-      <c r="AB28" s="169" t="s">
+      <c r="AB28" s="178" t="s">
         <v>95</v>
       </c>
       <c r="AC28" s="92"/>
@@ -26168,22 +26143,22 @@
     </row>
     <row r="29" spans="1:1026" ht="25" customHeight="1">
       <c r="A29" s="82" t="s">
-        <v>578</v>
+        <v>591</v>
       </c>
       <c r="B29" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D29" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E29" s="84" t="s">
         <v>155</v>
       </c>
       <c r="F29" s="82" t="s">
-        <v>613</v>
+        <v>592</v>
       </c>
       <c r="G29" s="85" t="s">
         <v>112</v>
@@ -26191,7 +26166,7 @@
       <c r="H29" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I29" s="169" t="s">
+      <c r="I29" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J29" s="104" t="s">
@@ -26210,7 +26185,7 @@
       <c r="O29" s="88"/>
       <c r="P29" s="107"/>
       <c r="Q29" s="54"/>
-      <c r="R29" s="169"/>
+      <c r="R29" s="110"/>
       <c r="S29" s="138"/>
       <c r="T29" s="93"/>
       <c r="U29" s="94"/>
@@ -26218,9 +26193,9 @@
       <c r="W29" s="95"/>
       <c r="X29" s="108"/>
       <c r="Y29" s="90"/>
-      <c r="Z29" s="109"/>
+      <c r="Z29" s="181"/>
       <c r="AA29" s="92"/>
-      <c r="AB29" s="169" t="s">
+      <c r="AB29" s="178" t="s">
         <v>107</v>
       </c>
       <c r="AC29" s="92"/>
@@ -27224,22 +27199,22 @@
     </row>
     <row r="30" spans="1:1026" ht="25" customHeight="1">
       <c r="A30" s="82" t="s">
-        <v>579</v>
+        <v>593</v>
       </c>
       <c r="B30" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C30" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D30" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E30" s="84" t="s">
         <v>160</v>
       </c>
       <c r="F30" s="82" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
       <c r="G30" s="85" t="s">
         <v>112</v>
@@ -27247,7 +27222,7 @@
       <c r="H30" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I30" s="169" t="s">
+      <c r="I30" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J30" s="104" t="s">
@@ -27266,7 +27241,7 @@
       <c r="O30" s="88"/>
       <c r="P30" s="107"/>
       <c r="Q30" s="54"/>
-      <c r="R30" s="169"/>
+      <c r="R30" s="110"/>
       <c r="S30" s="138"/>
       <c r="T30" s="93"/>
       <c r="U30" s="94"/>
@@ -27274,7 +27249,7 @@
       <c r="W30" s="95"/>
       <c r="X30" s="108"/>
       <c r="Y30" s="90"/>
-      <c r="Z30" s="109"/>
+      <c r="Z30" s="181"/>
       <c r="AA30" s="92"/>
       <c r="AB30" s="91" t="s">
         <v>116</v>
@@ -28280,22 +28255,22 @@
     </row>
     <row r="31" spans="1:1026" ht="25" customHeight="1">
       <c r="A31" s="82" t="s">
-        <v>580</v>
+        <v>595</v>
       </c>
       <c r="B31" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C31" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D31" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E31" s="84" t="s">
         <v>165</v>
       </c>
       <c r="F31" s="82" t="s">
-        <v>615</v>
+        <v>596</v>
       </c>
       <c r="G31" s="85" t="s">
         <v>112</v>
@@ -28303,7 +28278,7 @@
       <c r="H31" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I31" s="169" t="s">
+      <c r="I31" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J31" s="104" t="s">
@@ -28322,7 +28297,7 @@
       <c r="O31" s="88"/>
       <c r="P31" s="107"/>
       <c r="Q31" s="54"/>
-      <c r="R31" s="169"/>
+      <c r="R31" s="110"/>
       <c r="S31" s="138"/>
       <c r="T31" s="93"/>
       <c r="U31" s="94"/>
@@ -28330,7 +28305,7 @@
       <c r="W31" s="95"/>
       <c r="X31" s="108"/>
       <c r="Y31" s="90"/>
-      <c r="Z31" s="109"/>
+      <c r="Z31" s="181"/>
       <c r="AA31" s="92"/>
       <c r="AB31" s="91" t="s">
         <v>116</v>
@@ -29336,22 +29311,22 @@
     </row>
     <row r="32" spans="1:1026" ht="25" customHeight="1">
       <c r="A32" s="82" t="s">
-        <v>581</v>
+        <v>597</v>
       </c>
       <c r="B32" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C32" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D32" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E32" s="84" t="s">
         <v>170</v>
       </c>
       <c r="F32" s="82" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="G32" s="85" t="s">
         <v>112</v>
@@ -29359,7 +29334,7 @@
       <c r="H32" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I32" s="169" t="s">
+      <c r="I32" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J32" s="104" t="s">
@@ -29378,7 +29353,7 @@
       <c r="O32" s="88"/>
       <c r="P32" s="107"/>
       <c r="Q32" s="54"/>
-      <c r="R32" s="169"/>
+      <c r="R32" s="110"/>
       <c r="S32" s="138"/>
       <c r="T32" s="93"/>
       <c r="U32" s="94"/>
@@ -29386,7 +29361,7 @@
       <c r="W32" s="95"/>
       <c r="X32" s="108"/>
       <c r="Y32" s="90"/>
-      <c r="Z32" s="109"/>
+      <c r="Z32" s="181"/>
       <c r="AA32" s="92"/>
       <c r="AB32" s="91" t="s">
         <v>116</v>
@@ -30392,22 +30367,22 @@
     </row>
     <row r="33" spans="1:1026" ht="25" customHeight="1">
       <c r="A33" s="82" t="s">
-        <v>582</v>
+        <v>599</v>
       </c>
       <c r="B33" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C33" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D33" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E33" s="84" t="s">
         <v>175</v>
       </c>
       <c r="F33" s="82" t="s">
-        <v>617</v>
+        <v>600</v>
       </c>
       <c r="G33" s="85" t="s">
         <v>112</v>
@@ -30415,7 +30390,7 @@
       <c r="H33" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I33" s="169" t="s">
+      <c r="I33" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J33" s="104" t="s">
@@ -30434,7 +30409,7 @@
       <c r="O33" s="88"/>
       <c r="P33" s="107"/>
       <c r="Q33" s="54"/>
-      <c r="R33" s="169"/>
+      <c r="R33" s="110"/>
       <c r="S33" s="138"/>
       <c r="T33" s="93"/>
       <c r="U33" s="94"/>
@@ -30442,7 +30417,7 @@
       <c r="W33" s="95"/>
       <c r="X33" s="108"/>
       <c r="Y33" s="90"/>
-      <c r="Z33" s="109"/>
+      <c r="Z33" s="181"/>
       <c r="AA33" s="92"/>
       <c r="AB33" s="91" t="s">
         <v>116</v>
@@ -31448,22 +31423,22 @@
     </row>
     <row r="34" spans="1:1026" ht="25" customHeight="1">
       <c r="A34" s="82" t="s">
-        <v>583</v>
+        <v>601</v>
       </c>
       <c r="B34" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C34" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D34" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E34" s="84" t="s">
         <v>179</v>
       </c>
       <c r="F34" s="82" t="s">
-        <v>618</v>
+        <v>602</v>
       </c>
       <c r="G34" s="85" t="s">
         <v>112</v>
@@ -31471,7 +31446,7 @@
       <c r="H34" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I34" s="169" t="s">
+      <c r="I34" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J34" s="104" t="s">
@@ -31490,7 +31465,7 @@
       <c r="O34" s="88"/>
       <c r="P34" s="107"/>
       <c r="Q34" s="54"/>
-      <c r="R34" s="169"/>
+      <c r="R34" s="110"/>
       <c r="S34" s="138"/>
       <c r="T34" s="93"/>
       <c r="U34" s="94"/>
@@ -31498,7 +31473,7 @@
       <c r="W34" s="95"/>
       <c r="X34" s="108"/>
       <c r="Y34" s="90"/>
-      <c r="Z34" s="109"/>
+      <c r="Z34" s="181"/>
       <c r="AA34" s="92"/>
       <c r="AB34" s="91" t="s">
         <v>116</v>
@@ -32504,22 +32479,22 @@
     </row>
     <row r="35" spans="1:1026" ht="25" customHeight="1">
       <c r="A35" s="82" t="s">
-        <v>584</v>
+        <v>603</v>
       </c>
       <c r="B35" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C35" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D35" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E35" s="84" t="s">
         <v>183</v>
       </c>
       <c r="F35" s="82" t="s">
-        <v>619</v>
+        <v>604</v>
       </c>
       <c r="G35" s="85" t="s">
         <v>112</v>
@@ -32527,7 +32502,7 @@
       <c r="H35" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I35" s="169" t="s">
+      <c r="I35" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J35" s="104" t="s">
@@ -32546,7 +32521,7 @@
       <c r="O35" s="88"/>
       <c r="P35" s="107"/>
       <c r="Q35" s="54"/>
-      <c r="R35" s="169"/>
+      <c r="R35" s="110"/>
       <c r="S35" s="138"/>
       <c r="T35" s="93"/>
       <c r="U35" s="94"/>
@@ -32554,7 +32529,7 @@
       <c r="W35" s="95"/>
       <c r="X35" s="108"/>
       <c r="Y35" s="90"/>
-      <c r="Z35" s="109"/>
+      <c r="Z35" s="181"/>
       <c r="AA35" s="92"/>
       <c r="AB35" s="91" t="s">
         <v>116</v>
@@ -33560,22 +33535,22 @@
     </row>
     <row r="36" spans="1:1026" s="97" customFormat="1" ht="25" customHeight="1">
       <c r="A36" s="82" t="s">
-        <v>585</v>
+        <v>605</v>
       </c>
       <c r="B36" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C36" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D36" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E36" s="84" t="s">
         <v>187</v>
       </c>
       <c r="F36" s="82" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="G36" s="85" t="s">
         <v>112</v>
@@ -33583,7 +33558,7 @@
       <c r="H36" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I36" s="169" t="s">
+      <c r="I36" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J36" s="104" t="s">
@@ -33602,7 +33577,7 @@
       <c r="O36" s="88"/>
       <c r="P36" s="107"/>
       <c r="Q36" s="54"/>
-      <c r="R36" s="169"/>
+      <c r="R36" s="110"/>
       <c r="S36" s="138"/>
       <c r="T36" s="93"/>
       <c r="U36" s="94"/>
@@ -33610,7 +33585,7 @@
       <c r="W36" s="95"/>
       <c r="X36" s="108"/>
       <c r="Y36" s="90"/>
-      <c r="Z36" s="109"/>
+      <c r="Z36" s="181"/>
       <c r="AA36" s="92"/>
       <c r="AB36" s="91" t="s">
         <v>116</v>
@@ -33626,22 +33601,22 @@
     </row>
     <row r="37" spans="1:1026" s="97" customFormat="1" ht="25" customHeight="1">
       <c r="A37" s="82" t="s">
-        <v>586</v>
+        <v>607</v>
       </c>
       <c r="B37" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C37" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D37" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E37" s="84" t="s">
         <v>191</v>
       </c>
       <c r="F37" s="82" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
       <c r="G37" s="85" t="s">
         <v>112</v>
@@ -33649,7 +33624,7 @@
       <c r="H37" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I37" s="169" t="s">
+      <c r="I37" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J37" s="104" t="s">
@@ -33668,7 +33643,7 @@
       <c r="O37" s="88"/>
       <c r="P37" s="107"/>
       <c r="Q37" s="54"/>
-      <c r="R37" s="173"/>
+      <c r="R37" s="110"/>
       <c r="S37" s="138"/>
       <c r="T37" s="93"/>
       <c r="U37" s="94"/>
@@ -33676,7 +33651,7 @@
       <c r="W37" s="95"/>
       <c r="X37" s="108"/>
       <c r="Y37" s="90"/>
-      <c r="Z37" s="109"/>
+      <c r="Z37" s="181"/>
       <c r="AA37" s="92"/>
       <c r="AB37" s="91" t="s">
         <v>116</v>
@@ -33692,22 +33667,22 @@
     </row>
     <row r="38" spans="1:1026" s="97" customFormat="1" ht="25" customHeight="1">
       <c r="A38" s="82" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="B38" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C38" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D38" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E38" s="84" t="s">
         <v>195</v>
       </c>
       <c r="F38" s="82" t="s">
-        <v>622</v>
+        <v>610</v>
       </c>
       <c r="G38" s="85" t="s">
         <v>112</v>
@@ -33715,7 +33690,7 @@
       <c r="H38" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I38" s="169" t="s">
+      <c r="I38" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J38" s="104" t="s">
@@ -33734,7 +33709,7 @@
       <c r="O38" s="88"/>
       <c r="P38" s="107"/>
       <c r="Q38" s="54"/>
-      <c r="R38" s="169"/>
+      <c r="R38" s="110"/>
       <c r="S38" s="138"/>
       <c r="T38" s="93"/>
       <c r="U38" s="94"/>
@@ -33742,7 +33717,7 @@
       <c r="W38" s="95"/>
       <c r="X38" s="108"/>
       <c r="Y38" s="90"/>
-      <c r="Z38" s="109"/>
+      <c r="Z38" s="181"/>
       <c r="AA38" s="92"/>
       <c r="AB38" s="91" t="s">
         <v>116</v>
@@ -33758,22 +33733,22 @@
     </row>
     <row r="39" spans="1:1026" ht="25" customHeight="1">
       <c r="A39" s="82" t="s">
-        <v>588</v>
+        <v>611</v>
       </c>
       <c r="B39" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C39" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D39" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E39" s="84" t="s">
         <v>199</v>
       </c>
       <c r="F39" s="82" t="s">
-        <v>623</v>
+        <v>612</v>
       </c>
       <c r="G39" s="85" t="s">
         <v>112</v>
@@ -33781,7 +33756,7 @@
       <c r="H39" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I39" s="169" t="s">
+      <c r="I39" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J39" s="104" t="s">
@@ -33800,7 +33775,7 @@
       <c r="O39" s="88"/>
       <c r="P39" s="107"/>
       <c r="Q39" s="54"/>
-      <c r="R39" s="169"/>
+      <c r="R39" s="110"/>
       <c r="S39" s="138"/>
       <c r="T39" s="93"/>
       <c r="U39" s="94"/>
@@ -33808,7 +33783,7 @@
       <c r="W39" s="95"/>
       <c r="X39" s="108"/>
       <c r="Y39" s="90"/>
-      <c r="Z39" s="109"/>
+      <c r="Z39" s="181"/>
       <c r="AA39" s="92"/>
       <c r="AB39" s="91" t="s">
         <v>116</v>
@@ -34814,22 +34789,22 @@
     </row>
     <row r="40" spans="1:1026" ht="25" customHeight="1">
       <c r="A40" s="82" t="s">
-        <v>589</v>
+        <v>613</v>
       </c>
       <c r="B40" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C40" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D40" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E40" s="84" t="s">
         <v>203</v>
       </c>
       <c r="F40" s="82" t="s">
-        <v>624</v>
+        <v>614</v>
       </c>
       <c r="G40" s="85" t="s">
         <v>112</v>
@@ -34837,7 +34812,7 @@
       <c r="H40" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I40" s="169" t="s">
+      <c r="I40" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J40" s="104" t="s">
@@ -34856,7 +34831,7 @@
       <c r="O40" s="88"/>
       <c r="P40" s="107"/>
       <c r="Q40" s="54"/>
-      <c r="R40" s="169"/>
+      <c r="R40" s="110"/>
       <c r="S40" s="138"/>
       <c r="T40" s="93"/>
       <c r="U40" s="94"/>
@@ -34864,7 +34839,7 @@
       <c r="W40" s="95"/>
       <c r="X40" s="108"/>
       <c r="Y40" s="90"/>
-      <c r="Z40" s="109"/>
+      <c r="Z40" s="181"/>
       <c r="AA40" s="92"/>
       <c r="AB40" s="91" t="s">
         <v>116</v>
@@ -35870,22 +35845,22 @@
     </row>
     <row r="41" spans="1:1026" ht="25" customHeight="1">
       <c r="A41" s="82" t="s">
-        <v>590</v>
+        <v>615</v>
       </c>
       <c r="B41" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C41" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D41" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E41" s="84" t="s">
         <v>100</v>
       </c>
       <c r="F41" s="82" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
       <c r="G41" s="85" t="s">
         <v>112</v>
@@ -35893,7 +35868,7 @@
       <c r="H41" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I41" s="169" t="s">
+      <c r="I41" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J41" s="104" t="s">
@@ -35912,7 +35887,7 @@
       <c r="O41" s="88"/>
       <c r="P41" s="107"/>
       <c r="Q41" s="54"/>
-      <c r="R41" s="169"/>
+      <c r="R41" s="110"/>
       <c r="S41" s="138"/>
       <c r="T41" s="93"/>
       <c r="U41" s="94"/>
@@ -35920,7 +35895,7 @@
       <c r="W41" s="95"/>
       <c r="X41" s="108"/>
       <c r="Y41" s="90"/>
-      <c r="Z41" s="109"/>
+      <c r="Z41" s="181"/>
       <c r="AA41" s="92"/>
       <c r="AB41" s="91" t="s">
         <v>116</v>
@@ -36926,22 +36901,22 @@
     </row>
     <row r="42" spans="1:1026" ht="25" customHeight="1">
       <c r="A42" s="82" t="s">
-        <v>591</v>
+        <v>617</v>
       </c>
       <c r="B42" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D42" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E42" s="84" t="s">
         <v>215</v>
       </c>
       <c r="F42" s="82" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="G42" s="85" t="s">
         <v>112</v>
@@ -36949,7 +36924,7 @@
       <c r="H42" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I42" s="169" t="s">
+      <c r="I42" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J42" s="104" t="s">
@@ -36968,7 +36943,7 @@
       <c r="O42" s="88"/>
       <c r="P42" s="107"/>
       <c r="Q42" s="54"/>
-      <c r="R42" s="169"/>
+      <c r="R42" s="110"/>
       <c r="S42" s="138"/>
       <c r="T42" s="93"/>
       <c r="U42" s="94"/>
@@ -36976,8 +36951,8 @@
       <c r="W42" s="95"/>
       <c r="X42" s="108"/>
       <c r="Y42" s="90"/>
-      <c r="Z42" s="109" t="s">
-        <v>638</v>
+      <c r="Z42" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA42" s="92"/>
       <c r="AB42" s="91" t="s">
@@ -37984,22 +37959,22 @@
     </row>
     <row r="43" spans="1:1026" ht="25" customHeight="1">
       <c r="A43" s="82" t="s">
-        <v>592</v>
+        <v>619</v>
       </c>
       <c r="B43" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C43" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D43" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E43" s="84" t="s">
         <v>219</v>
       </c>
       <c r="F43" s="82" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="G43" s="85" t="s">
         <v>112</v>
@@ -38007,7 +37982,7 @@
       <c r="H43" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I43" s="169" t="s">
+      <c r="I43" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J43" s="104" t="s">
@@ -38026,7 +38001,7 @@
       <c r="O43" s="88"/>
       <c r="P43" s="107"/>
       <c r="Q43" s="54"/>
-      <c r="R43" s="169"/>
+      <c r="R43" s="110"/>
       <c r="S43" s="138"/>
       <c r="T43" s="93"/>
       <c r="U43" s="94"/>
@@ -38034,8 +38009,8 @@
       <c r="W43" s="95"/>
       <c r="X43" s="108"/>
       <c r="Y43" s="90"/>
-      <c r="Z43" s="109" t="s">
-        <v>638</v>
+      <c r="Z43" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA43" s="92"/>
       <c r="AB43" s="91" t="s">
@@ -39042,22 +39017,22 @@
     </row>
     <row r="44" spans="1:1026" ht="25" customHeight="1">
       <c r="A44" s="82" t="s">
-        <v>593</v>
+        <v>621</v>
       </c>
       <c r="B44" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C44" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D44" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E44" s="84" t="s">
         <v>222</v>
       </c>
       <c r="F44" s="82" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="G44" s="85" t="s">
         <v>112</v>
@@ -39065,7 +39040,7 @@
       <c r="H44" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I44" s="169" t="s">
+      <c r="I44" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J44" s="104" t="s">
@@ -39084,7 +39059,7 @@
       <c r="O44" s="88"/>
       <c r="P44" s="107"/>
       <c r="Q44" s="54"/>
-      <c r="R44" s="169"/>
+      <c r="R44" s="110"/>
       <c r="S44" s="138"/>
       <c r="T44" s="93"/>
       <c r="U44" s="94"/>
@@ -39092,8 +39067,8 @@
       <c r="W44" s="95"/>
       <c r="X44" s="108"/>
       <c r="Y44" s="90"/>
-      <c r="Z44" s="109" t="s">
-        <v>638</v>
+      <c r="Z44" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA44" s="92"/>
       <c r="AB44" s="91" t="s">
@@ -40100,22 +40075,22 @@
     </row>
     <row r="45" spans="1:1026" ht="25" customHeight="1">
       <c r="A45" s="82" t="s">
-        <v>594</v>
+        <v>623</v>
       </c>
       <c r="B45" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C45" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D45" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E45" s="84" t="s">
         <v>226</v>
       </c>
       <c r="F45" s="82" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="G45" s="85" t="s">
         <v>112</v>
@@ -40123,7 +40098,7 @@
       <c r="H45" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I45" s="169" t="s">
+      <c r="I45" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J45" s="104" t="s">
@@ -40142,7 +40117,7 @@
       <c r="O45" s="88"/>
       <c r="P45" s="107"/>
       <c r="Q45" s="54"/>
-      <c r="R45" s="169"/>
+      <c r="R45" s="110"/>
       <c r="S45" s="138"/>
       <c r="T45" s="93"/>
       <c r="U45" s="94"/>
@@ -40150,8 +40125,8 @@
       <c r="W45" s="95"/>
       <c r="X45" s="108"/>
       <c r="Y45" s="90"/>
-      <c r="Z45" s="109" t="s">
-        <v>638</v>
+      <c r="Z45" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA45" s="92"/>
       <c r="AB45" s="91" t="s">
@@ -41158,22 +41133,22 @@
     </row>
     <row r="46" spans="1:1026" ht="25" customHeight="1">
       <c r="A46" s="82" t="s">
-        <v>595</v>
+        <v>625</v>
       </c>
       <c r="B46" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C46" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D46" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E46" s="84" t="s">
         <v>230</v>
       </c>
       <c r="F46" s="82" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="G46" s="85" t="s">
         <v>112</v>
@@ -41181,7 +41156,7 @@
       <c r="H46" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I46" s="169" t="s">
+      <c r="I46" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J46" s="104" t="s">
@@ -41200,7 +41175,7 @@
       <c r="O46" s="88"/>
       <c r="P46" s="107"/>
       <c r="Q46" s="54"/>
-      <c r="R46" s="169"/>
+      <c r="R46" s="110"/>
       <c r="S46" s="138"/>
       <c r="T46" s="93"/>
       <c r="U46" s="94"/>
@@ -41208,8 +41183,8 @@
       <c r="W46" s="95"/>
       <c r="X46" s="108"/>
       <c r="Y46" s="90"/>
-      <c r="Z46" s="109" t="s">
-        <v>638</v>
+      <c r="Z46" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA46" s="92"/>
       <c r="AB46" s="91" t="s">
@@ -42216,22 +42191,22 @@
     </row>
     <row r="47" spans="1:1026" ht="25" customHeight="1">
       <c r="A47" s="82" t="s">
-        <v>596</v>
+        <v>627</v>
       </c>
       <c r="B47" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C47" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D47" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E47" s="84" t="s">
         <v>234</v>
       </c>
       <c r="F47" s="82" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="G47" s="85" t="s">
         <v>112</v>
@@ -42239,7 +42214,7 @@
       <c r="H47" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I47" s="169" t="s">
+      <c r="I47" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J47" s="104" t="s">
@@ -42258,7 +42233,7 @@
       <c r="O47" s="88"/>
       <c r="P47" s="107"/>
       <c r="Q47" s="54"/>
-      <c r="R47" s="169"/>
+      <c r="R47" s="110"/>
       <c r="S47" s="138"/>
       <c r="T47" s="93"/>
       <c r="U47" s="94"/>
@@ -42266,8 +42241,8 @@
       <c r="W47" s="95"/>
       <c r="X47" s="108"/>
       <c r="Y47" s="90"/>
-      <c r="Z47" s="109" t="s">
-        <v>638</v>
+      <c r="Z47" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA47" s="92"/>
       <c r="AB47" s="91" t="s">
@@ -43274,22 +43249,22 @@
     </row>
     <row r="48" spans="1:1026" ht="25" customHeight="1">
       <c r="A48" s="82" t="s">
-        <v>597</v>
+        <v>629</v>
       </c>
       <c r="B48" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C48" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D48" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E48" s="84" t="s">
         <v>238</v>
       </c>
       <c r="F48" s="82" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="G48" s="85" t="s">
         <v>112</v>
@@ -43297,7 +43272,7 @@
       <c r="H48" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I48" s="169" t="s">
+      <c r="I48" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J48" s="104" t="s">
@@ -43316,7 +43291,7 @@
       <c r="O48" s="88"/>
       <c r="P48" s="107"/>
       <c r="Q48" s="54"/>
-      <c r="R48" s="169"/>
+      <c r="R48" s="110"/>
       <c r="S48" s="138"/>
       <c r="T48" s="93"/>
       <c r="U48" s="94"/>
@@ -43324,8 +43299,8 @@
       <c r="W48" s="95"/>
       <c r="X48" s="108"/>
       <c r="Y48" s="90"/>
-      <c r="Z48" s="109" t="s">
-        <v>638</v>
+      <c r="Z48" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA48" s="92"/>
       <c r="AB48" s="91" t="s">
@@ -44332,22 +44307,22 @@
     </row>
     <row r="49" spans="1:1026" ht="25" customHeight="1">
       <c r="A49" s="82" t="s">
-        <v>598</v>
+        <v>631</v>
       </c>
       <c r="B49" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C49" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D49" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E49" s="84" t="s">
         <v>242</v>
       </c>
       <c r="F49" s="82" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G49" s="85" t="s">
         <v>112</v>
@@ -44355,7 +44330,7 @@
       <c r="H49" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I49" s="169" t="s">
+      <c r="I49" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J49" s="104" t="s">
@@ -44374,7 +44349,7 @@
       <c r="O49" s="88"/>
       <c r="P49" s="107"/>
       <c r="Q49" s="54"/>
-      <c r="R49" s="169"/>
+      <c r="R49" s="110"/>
       <c r="S49" s="138"/>
       <c r="T49" s="93"/>
       <c r="U49" s="94"/>
@@ -44382,8 +44357,8 @@
       <c r="W49" s="95"/>
       <c r="X49" s="108"/>
       <c r="Y49" s="90"/>
-      <c r="Z49" s="109" t="s">
-        <v>638</v>
+      <c r="Z49" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA49" s="92"/>
       <c r="AB49" s="91" t="s">
@@ -45390,16 +45365,16 @@
     </row>
     <row r="50" spans="1:1026" s="99" customFormat="1" ht="25" customHeight="1">
       <c r="A50" s="82" t="s">
-        <v>599</v>
+        <v>633</v>
       </c>
       <c r="B50" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C50" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D50" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E50" s="84" t="s">
         <v>246</v>
@@ -45413,7 +45388,7 @@
       <c r="H50" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I50" s="169" t="s">
+      <c r="I50" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J50" s="104" t="s">
@@ -45432,7 +45407,7 @@
       <c r="O50" s="88"/>
       <c r="P50" s="107"/>
       <c r="Q50" s="54"/>
-      <c r="R50" s="169"/>
+      <c r="R50" s="110"/>
       <c r="S50" s="138"/>
       <c r="T50" s="93"/>
       <c r="U50" s="94"/>
@@ -45440,8 +45415,8 @@
       <c r="W50" s="95"/>
       <c r="X50" s="108"/>
       <c r="Y50" s="90"/>
-      <c r="Z50" s="109" t="s">
-        <v>638</v>
+      <c r="Z50" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA50" s="92"/>
       <c r="AB50" s="91" t="s">
@@ -45458,22 +45433,22 @@
     </row>
     <row r="51" spans="1:1026" ht="25" customHeight="1">
       <c r="A51" s="82" t="s">
-        <v>600</v>
+        <v>635</v>
       </c>
       <c r="B51" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C51" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D51" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E51" s="84" t="s">
         <v>246</v>
       </c>
       <c r="F51" s="82" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="G51" s="85" t="s">
         <v>112</v>
@@ -45481,7 +45456,7 @@
       <c r="H51" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I51" s="169" t="s">
+      <c r="I51" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J51" s="104" t="s">
@@ -45500,7 +45475,7 @@
       <c r="O51" s="88"/>
       <c r="P51" s="107"/>
       <c r="Q51" s="54"/>
-      <c r="R51" s="170"/>
+      <c r="R51" s="110"/>
       <c r="S51" s="138"/>
       <c r="T51" s="93"/>
       <c r="U51" s="94"/>
@@ -45508,8 +45483,8 @@
       <c r="W51" s="95"/>
       <c r="X51" s="108"/>
       <c r="Y51" s="90"/>
-      <c r="Z51" s="109" t="s">
-        <v>638</v>
+      <c r="Z51" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA51" s="92"/>
       <c r="AB51" s="91" t="s">
@@ -46516,22 +46491,22 @@
     </row>
     <row r="52" spans="1:1026" ht="25" customHeight="1">
       <c r="A52" s="82" t="s">
-        <v>601</v>
+        <v>637</v>
       </c>
       <c r="B52" s="83" t="s">
         <v>90</v>
       </c>
       <c r="C52" s="84" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D52" s="84" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E52" s="84" t="s">
         <v>246</v>
       </c>
       <c r="F52" s="82" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="G52" s="85" t="s">
         <v>112</v>
@@ -46539,7 +46514,7 @@
       <c r="H52" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="I52" s="169" t="s">
+      <c r="I52" s="178" t="s">
         <v>92</v>
       </c>
       <c r="J52" s="104" t="s">
@@ -46558,7 +46533,7 @@
       <c r="O52" s="88"/>
       <c r="P52" s="107"/>
       <c r="Q52" s="54"/>
-      <c r="R52" s="174"/>
+      <c r="R52" s="110"/>
       <c r="S52" s="138"/>
       <c r="T52" s="93"/>
       <c r="U52" s="94"/>
@@ -46566,8 +46541,8 @@
       <c r="W52" s="95"/>
       <c r="X52" s="108"/>
       <c r="Y52" s="90"/>
-      <c r="Z52" s="109" t="s">
-        <v>638</v>
+      <c r="Z52" s="181" t="s">
+        <v>567</v>
       </c>
       <c r="AA52" s="92"/>
       <c r="AB52" s="91" t="s">
@@ -47573,15 +47548,15 @@
       <c r="AML52"/>
     </row>
     <row r="53" spans="1:1026" ht="25" customHeight="1">
-      <c r="A53" s="82"/>
+      <c r="A53" s="98"/>
       <c r="B53" s="83"/>
       <c r="C53" s="84"/>
       <c r="D53" s="84"/>
       <c r="E53" s="84"/>
-      <c r="F53" s="82"/>
+      <c r="F53" s="89"/>
       <c r="G53" s="85"/>
       <c r="H53" s="86"/>
-      <c r="I53" s="169"/>
+      <c r="I53" s="103"/>
       <c r="J53" s="104"/>
       <c r="K53" s="105"/>
       <c r="L53" s="105"/>
@@ -47590,7 +47565,7 @@
       <c r="O53" s="88"/>
       <c r="P53" s="107"/>
       <c r="Q53" s="54"/>
-      <c r="R53" s="174"/>
+      <c r="R53" s="110"/>
       <c r="S53" s="138"/>
       <c r="T53" s="93"/>
       <c r="U53" s="94"/>
@@ -48601,15 +48576,15 @@
       <c r="AML53"/>
     </row>
     <row r="54" spans="1:1026" ht="25" customHeight="1">
-      <c r="A54" s="82"/>
+      <c r="A54" s="98"/>
       <c r="B54" s="83"/>
       <c r="C54" s="84"/>
       <c r="D54" s="84"/>
       <c r="E54" s="84"/>
-      <c r="F54" s="82"/>
+      <c r="F54" s="89"/>
       <c r="G54" s="85"/>
       <c r="H54" s="86"/>
-      <c r="I54" s="169"/>
+      <c r="I54" s="103"/>
       <c r="J54" s="104"/>
       <c r="K54" s="105"/>
       <c r="L54" s="105"/>
@@ -48618,7 +48593,7 @@
       <c r="O54" s="88"/>
       <c r="P54" s="107"/>
       <c r="Q54" s="54"/>
-      <c r="R54" s="174"/>
+      <c r="R54" s="110"/>
       <c r="S54" s="138"/>
       <c r="T54" s="93"/>
       <c r="U54" s="94"/>
@@ -49629,15 +49604,15 @@
       <c r="AML54"/>
     </row>
     <row r="55" spans="1:1026" ht="25" customHeight="1">
-      <c r="A55" s="82"/>
+      <c r="A55" s="98"/>
       <c r="B55" s="83"/>
       <c r="C55" s="84"/>
       <c r="D55" s="84"/>
       <c r="E55" s="84"/>
-      <c r="F55" s="82"/>
+      <c r="F55" s="89"/>
       <c r="G55" s="85"/>
       <c r="H55" s="86"/>
-      <c r="I55" s="169"/>
+      <c r="I55" s="103"/>
       <c r="J55" s="104"/>
       <c r="K55" s="105"/>
       <c r="L55" s="105"/>
@@ -49646,7 +49621,7 @@
       <c r="O55" s="88"/>
       <c r="P55" s="107"/>
       <c r="Q55" s="54"/>
-      <c r="R55" s="174"/>
+      <c r="R55" s="110"/>
       <c r="S55" s="138"/>
       <c r="T55" s="93"/>
       <c r="U55" s="94"/>
@@ -50657,15 +50632,15 @@
       <c r="AML55"/>
     </row>
     <row r="56" spans="1:1026" ht="25" customHeight="1">
-      <c r="A56" s="82"/>
+      <c r="A56" s="98"/>
       <c r="B56" s="83"/>
       <c r="C56" s="84"/>
       <c r="D56" s="84"/>
       <c r="E56" s="84"/>
-      <c r="F56" s="82"/>
+      <c r="F56" s="89"/>
       <c r="G56" s="85"/>
       <c r="H56" s="86"/>
-      <c r="I56" s="169"/>
+      <c r="I56" s="103"/>
       <c r="J56" s="104"/>
       <c r="K56" s="105"/>
       <c r="L56" s="105"/>
@@ -50674,7 +50649,7 @@
       <c r="O56" s="88"/>
       <c r="P56" s="107"/>
       <c r="Q56" s="54"/>
-      <c r="R56" s="174"/>
+      <c r="R56" s="110"/>
       <c r="S56" s="138"/>
       <c r="T56" s="93"/>
       <c r="U56" s="94"/>
@@ -51685,15 +51660,15 @@
       <c r="AML56"/>
     </row>
     <row r="57" spans="1:1026" ht="25" customHeight="1">
-      <c r="A57" s="82"/>
+      <c r="A57" s="98"/>
       <c r="B57" s="83"/>
       <c r="C57" s="84"/>
       <c r="D57" s="84"/>
       <c r="E57" s="84"/>
-      <c r="F57" s="82"/>
+      <c r="F57" s="89"/>
       <c r="G57" s="85"/>
       <c r="H57" s="86"/>
-      <c r="I57" s="169"/>
+      <c r="I57" s="103"/>
       <c r="J57" s="104"/>
       <c r="K57" s="105"/>
       <c r="L57" s="105"/>
@@ -51702,7 +51677,7 @@
       <c r="O57" s="88"/>
       <c r="P57" s="107"/>
       <c r="Q57" s="54"/>
-      <c r="R57" s="174"/>
+      <c r="R57" s="110"/>
       <c r="S57" s="138"/>
       <c r="T57" s="93"/>
       <c r="U57" s="94"/>
@@ -52713,15 +52688,15 @@
       <c r="AML57"/>
     </row>
     <row r="58" spans="1:1026" ht="25" customHeight="1">
-      <c r="A58" s="82"/>
+      <c r="A58" s="98"/>
       <c r="B58" s="83"/>
       <c r="C58" s="84"/>
       <c r="D58" s="84"/>
-      <c r="E58" s="166"/>
-      <c r="F58" s="82"/>
+      <c r="E58" s="84"/>
+      <c r="F58" s="89"/>
       <c r="G58" s="85"/>
       <c r="H58" s="86"/>
-      <c r="I58" s="169"/>
+      <c r="I58" s="103"/>
       <c r="J58" s="104"/>
       <c r="K58" s="105"/>
       <c r="L58" s="105"/>
@@ -52730,7 +52705,7 @@
       <c r="O58" s="88"/>
       <c r="P58" s="107"/>
       <c r="Q58" s="54"/>
-      <c r="R58" s="174"/>
+      <c r="R58" s="110"/>
       <c r="S58" s="138"/>
       <c r="T58" s="93"/>
       <c r="U58" s="94"/>
@@ -53741,15 +53716,15 @@
       <c r="AML58"/>
     </row>
     <row r="59" spans="1:1026" ht="25" customHeight="1">
-      <c r="A59" s="82"/>
+      <c r="A59" s="98"/>
       <c r="B59" s="83"/>
       <c r="C59" s="84"/>
       <c r="D59" s="84"/>
-      <c r="E59" s="166"/>
-      <c r="F59" s="82"/>
+      <c r="E59" s="84"/>
+      <c r="F59" s="89"/>
       <c r="G59" s="85"/>
       <c r="H59" s="86"/>
-      <c r="I59" s="169"/>
+      <c r="I59" s="103"/>
       <c r="J59" s="104"/>
       <c r="K59" s="105"/>
       <c r="L59" s="105"/>
@@ -53758,7 +53733,7 @@
       <c r="O59" s="88"/>
       <c r="P59" s="107"/>
       <c r="Q59" s="54"/>
-      <c r="R59" s="174"/>
+      <c r="R59" s="110"/>
       <c r="S59" s="138"/>
       <c r="T59" s="93"/>
       <c r="U59" s="94"/>
@@ -54769,15 +54744,15 @@
       <c r="AML59"/>
     </row>
     <row r="60" spans="1:1026" ht="25" customHeight="1">
-      <c r="A60" s="82"/>
+      <c r="A60" s="98"/>
       <c r="B60" s="83"/>
       <c r="C60" s="84"/>
       <c r="D60" s="84"/>
-      <c r="E60" s="166"/>
-      <c r="F60" s="82"/>
+      <c r="E60" s="84"/>
+      <c r="F60" s="89"/>
       <c r="G60" s="85"/>
       <c r="H60" s="86"/>
-      <c r="I60" s="169"/>
+      <c r="I60" s="103"/>
       <c r="J60" s="104"/>
       <c r="K60" s="105"/>
       <c r="L60" s="105"/>
@@ -54786,7 +54761,7 @@
       <c r="O60" s="88"/>
       <c r="P60" s="107"/>
       <c r="Q60" s="54"/>
-      <c r="R60" s="174"/>
+      <c r="R60" s="110"/>
       <c r="S60" s="138"/>
       <c r="T60" s="93"/>
       <c r="U60" s="94"/>
@@ -55801,7 +55776,7 @@
       <c r="B61" s="83"/>
       <c r="C61" s="84"/>
       <c r="D61" s="84"/>
-      <c r="E61" s="167"/>
+      <c r="E61" s="84"/>
       <c r="F61" s="89"/>
       <c r="G61" s="85"/>
       <c r="H61" s="86"/>
@@ -56829,7 +56804,7 @@
       <c r="B62" s="83"/>
       <c r="C62" s="84"/>
       <c r="D62" s="84"/>
-      <c r="E62" s="167"/>
+      <c r="E62" s="84"/>
       <c r="F62" s="89"/>
       <c r="G62" s="85"/>
       <c r="H62" s="86"/>
@@ -57857,7 +57832,7 @@
       <c r="B63" s="83"/>
       <c r="C63" s="84"/>
       <c r="D63" s="84"/>
-      <c r="E63" s="168"/>
+      <c r="E63" s="84"/>
       <c r="F63" s="89"/>
       <c r="G63" s="85"/>
       <c r="H63" s="86"/>
@@ -57895,7 +57870,7 @@
       <c r="B64" s="83"/>
       <c r="C64" s="84"/>
       <c r="D64" s="84"/>
-      <c r="E64" s="168"/>
+      <c r="E64" s="84"/>
       <c r="F64" s="89"/>
       <c r="G64" s="85"/>
       <c r="H64" s="86"/>
@@ -70522,6 +70497,12 @@
           </x14:formula1>
           <xm:sqref>H15:H394</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!$H$3:$H$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>I15:I394</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$I$3:$I$4</xm:f>
@@ -70582,35 +70563,29 @@
           </x14:formula1>
           <xm:sqref>J15:J394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B0AA3873-BAA4-344B-8D69-5363B8ABD105}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!$C$3:$C$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>D15:D395</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F5EFDFDE-5DD6-274F-8F07-5A678B18218E}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!$B$3:$B$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>C15:C394</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000F000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$N$3:$N$40</xm:f>
           </x14:formula1>
           <xm:sqref>R15:R394</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F5EFDFDE-5DD6-274F-8F07-5A678B18218E}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!$B$3:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C15:C394</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B0AA3873-BAA4-344B-8D69-5363B8ABD105}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!$C$3:$C$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D15:D395</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
-            <xm:f>'Drop down lists'!$D$3:$D$53</xm:f>
+            <xm:f>'Drop down lists'!$D$3:$D$52</xm:f>
           </x14:formula1>
-          <xm:sqref>E15:E60 E65:E395</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!$H$3:$H$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>I30:I394 I15:I28</xm:sqref>
+          <xm:sqref>E15:E395</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -70626,7 +70601,7 @@
   <dimension ref="A2:AM203"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N40"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -70646,7 +70621,7 @@
         <v>58</v>
       </c>
       <c r="C2" s="70" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D2" s="70" t="s">
         <v>59</v>
@@ -70718,13 +70693,13 @@
         <v>88</v>
       </c>
       <c r="B3" s="145" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C3" s="145" t="s">
-        <v>538</v>
+        <v>554</v>
       </c>
       <c r="D3" s="145" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E3" s="144" t="s">
         <v>89</v>
@@ -70771,10 +70746,10 @@
         <v>99</v>
       </c>
       <c r="B4" s="145" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C4" s="145" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="D4" s="145" t="s">
         <v>100</v>
@@ -70822,10 +70797,10 @@
     <row r="5" spans="1:39">
       <c r="A5" s="152"/>
       <c r="B5" s="145" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C5" s="145" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D5" s="145" t="s">
         <v>130</v>
@@ -70864,11 +70839,11 @@
     </row>
     <row r="6" spans="1:39">
       <c r="A6" s="152"/>
-      <c r="B6" s="145" t="s">
-        <v>547</v>
+      <c r="B6" s="160" t="s">
+        <v>543</v>
       </c>
       <c r="C6" s="145" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="D6" s="145" t="s">
         <v>135</v>
@@ -70900,8 +70875,8 @@
     </row>
     <row r="7" spans="1:39">
       <c r="A7" s="152"/>
-      <c r="B7" s="160" t="s">
-        <v>548</v>
+      <c r="C7" s="145" t="s">
+        <v>545</v>
       </c>
       <c r="D7" s="145" t="s">
         <v>111</v>
@@ -70931,9 +70906,8 @@
     <row r="8" spans="1:39">
       <c r="A8" s="152"/>
       <c r="B8" s="155"/>
-      <c r="C8" s="155"/>
       <c r="D8" s="145" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F8" s="146" t="s">
         <v>131</v>
@@ -70957,7 +70931,7 @@
     <row r="9" spans="1:39">
       <c r="A9" s="152"/>
       <c r="B9" s="153"/>
-      <c r="C9" s="153"/>
+      <c r="C9" s="155"/>
       <c r="D9" s="145" t="s">
         <v>140</v>
       </c>
@@ -70983,9 +70957,9 @@
     <row r="10" spans="1:39">
       <c r="A10" s="152"/>
       <c r="B10" s="142"/>
-      <c r="C10" s="142"/>
+      <c r="C10" s="153"/>
       <c r="D10" s="145" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="F10" s="146" t="s">
         <v>141</v>
@@ -71008,6 +70982,7 @@
     </row>
     <row r="11" spans="1:39">
       <c r="A11" s="152"/>
+      <c r="C11" s="142"/>
       <c r="D11" s="145" t="s">
         <v>520</v>
       </c>
@@ -71033,7 +71008,6 @@
     <row r="12" spans="1:39">
       <c r="A12" s="152"/>
       <c r="B12" s="156"/>
-      <c r="C12" s="156"/>
       <c r="D12" s="145" t="s">
         <v>521</v>
       </c>
@@ -71162,8 +71136,9 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="152"/>
+      <c r="C17" s="156"/>
       <c r="D17" s="145" t="s">
-        <v>526</v>
+        <v>145</v>
       </c>
       <c r="F17" s="146" t="s">
         <v>176</v>
@@ -71184,7 +71159,7 @@
     <row r="18" spans="1:17">
       <c r="A18" s="152"/>
       <c r="D18" s="145" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F18" s="146" t="s">
         <v>180</v>
@@ -71205,9 +71180,8 @@
     <row r="19" spans="1:17">
       <c r="A19" s="152"/>
       <c r="B19" s="156"/>
-      <c r="C19" s="156"/>
       <c r="D19" s="145" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F19" s="146" t="s">
         <v>184</v>
@@ -71230,7 +71204,7 @@
       <c r="B20" s="156"/>
       <c r="C20" s="156"/>
       <c r="D20" s="145" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="F20" s="146" t="s">
         <v>188</v>
@@ -71253,7 +71227,7 @@
       <c r="B21" s="156"/>
       <c r="C21" s="156"/>
       <c r="D21" s="145" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F21" s="146" t="s">
         <v>192</v>
@@ -71276,7 +71250,7 @@
       <c r="B22" s="156"/>
       <c r="C22" s="156"/>
       <c r="D22" s="145" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="F22" s="146" t="s">
         <v>196</v>
@@ -71299,7 +71273,7 @@
       <c r="B23" s="156"/>
       <c r="C23" s="156"/>
       <c r="D23" s="145" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="F23" s="146" t="s">
         <v>200</v>
@@ -71319,7 +71293,7 @@
       <c r="B24" s="156"/>
       <c r="C24" s="156"/>
       <c r="D24" s="145" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F24" s="146" t="s">
         <v>204</v>
@@ -71339,7 +71313,7 @@
       <c r="B25" s="156"/>
       <c r="C25" s="156"/>
       <c r="D25" s="145" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F25" s="146" t="s">
         <v>208</v>
@@ -71348,7 +71322,7 @@
         <v>209</v>
       </c>
       <c r="N25" s="165" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="Q25" s="148">
         <v>22</v>
@@ -71359,7 +71333,7 @@
       <c r="B26" s="156"/>
       <c r="C26" s="156"/>
       <c r="D26" s="145" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F26" s="146" t="s">
         <v>212</v>
@@ -71379,7 +71353,7 @@
       <c r="B27" s="156"/>
       <c r="C27" s="156"/>
       <c r="D27" s="145" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F27" s="146" t="s">
         <v>216</v>
@@ -71399,7 +71373,7 @@
       <c r="B28" s="156"/>
       <c r="C28" s="156"/>
       <c r="D28" s="145" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F28" s="146" t="s">
         <v>220</v>
@@ -71419,7 +71393,7 @@
       <c r="B29" s="156"/>
       <c r="C29" s="156"/>
       <c r="D29" s="145" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="F29" s="146" t="s">
         <v>223</v>
@@ -71439,7 +71413,7 @@
       <c r="B30" s="156"/>
       <c r="C30" s="156"/>
       <c r="D30" s="145" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="F30" s="146" t="s">
         <v>227</v>
@@ -71458,7 +71432,7 @@
       <c r="B31" s="156"/>
       <c r="C31" s="156"/>
       <c r="D31" s="145" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="F31" s="146" t="s">
         <v>231</v>
@@ -71477,7 +71451,7 @@
       <c r="B32" s="156"/>
       <c r="C32" s="156"/>
       <c r="D32" s="145" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F32" s="146" t="s">
         <v>235</v>
@@ -71496,7 +71470,7 @@
       <c r="B33" s="156"/>
       <c r="C33" s="156"/>
       <c r="D33" s="145" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="F33" s="146" t="s">
         <v>239</v>
@@ -71515,7 +71489,7 @@
       <c r="B34" s="156"/>
       <c r="C34" s="156"/>
       <c r="D34" s="145" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F34" s="146" t="s">
         <v>243</v>
@@ -71534,7 +71508,7 @@
       <c r="B35" s="156"/>
       <c r="C35" s="156"/>
       <c r="D35" s="145" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F35" s="146" t="s">
         <v>247</v>
@@ -71553,7 +71527,7 @@
       <c r="B36" s="156"/>
       <c r="C36" s="156"/>
       <c r="D36" s="145" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="F36" s="146" t="s">
         <v>251</v>
@@ -71572,7 +71546,7 @@
       <c r="B37" s="156"/>
       <c r="C37" s="156"/>
       <c r="D37" s="145" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="F37" s="146" t="s">
         <v>255</v>
@@ -71591,7 +71565,7 @@
       <c r="B38" s="156"/>
       <c r="C38" s="156"/>
       <c r="D38" s="145" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="F38" s="146" t="s">
         <v>259</v>
@@ -71607,8 +71581,9 @@
       </c>
     </row>
     <row r="39" spans="2:17">
+      <c r="C39" s="156"/>
       <c r="D39" s="145" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F39" s="146" t="s">
         <v>263</v>
@@ -71625,7 +71600,7 @@
     </row>
     <row r="40" spans="2:17">
       <c r="D40" s="145" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="F40" s="146" t="s">
         <v>267</v>
@@ -71642,7 +71617,7 @@
     </row>
     <row r="41" spans="2:17">
       <c r="D41" s="145" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="F41" s="146" t="s">
         <v>271</v>
@@ -71656,7 +71631,7 @@
     </row>
     <row r="42" spans="2:17">
       <c r="D42" s="145" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F42" s="146" t="s">
         <v>273</v>
@@ -71670,7 +71645,7 @@
     </row>
     <row r="43" spans="2:17">
       <c r="D43" s="145" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F43" s="146" t="s">
         <v>275</v>
@@ -71684,7 +71659,7 @@
     </row>
     <row r="44" spans="2:17">
       <c r="D44" s="145" t="s">
-        <v>254</v>
+        <v>393</v>
       </c>
       <c r="F44" s="146" t="s">
         <v>277</v>
@@ -71698,7 +71673,7 @@
     </row>
     <row r="45" spans="2:17">
       <c r="D45" s="145" t="s">
-        <v>393</v>
+        <v>258</v>
       </c>
       <c r="F45" s="146" t="s">
         <v>279</v>
@@ -71712,7 +71687,7 @@
     </row>
     <row r="46" spans="2:17">
       <c r="D46" s="145" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="F46" s="146" t="s">
         <v>281</v>
@@ -71726,7 +71701,7 @@
     </row>
     <row r="47" spans="2:17">
       <c r="D47" s="145" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="F47" s="146" t="s">
         <v>283</v>
@@ -71740,7 +71715,7 @@
     </row>
     <row r="48" spans="2:17">
       <c r="D48" s="145" t="s">
-        <v>266</v>
+        <v>392</v>
       </c>
       <c r="F48" s="146" t="s">
         <v>285</v>
@@ -71754,7 +71729,7 @@
     </row>
     <row r="49" spans="4:17">
       <c r="D49" s="145" t="s">
-        <v>392</v>
+        <v>270</v>
       </c>
       <c r="F49" s="146" t="s">
         <v>287</v>
@@ -71767,8 +71742,8 @@
       </c>
     </row>
     <row r="50" spans="4:17">
-      <c r="D50" s="145" t="s">
-        <v>270</v>
+      <c r="D50" s="148" t="s">
+        <v>394</v>
       </c>
       <c r="F50" s="146" t="s">
         <v>289</v>
@@ -71782,7 +71757,7 @@
     </row>
     <row r="51" spans="4:17">
       <c r="D51" s="148" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="F51" s="146" t="s">
         <v>291</v>
@@ -71796,7 +71771,7 @@
     </row>
     <row r="52" spans="4:17">
       <c r="D52" s="148" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F52" s="146" t="s">
         <v>293</v>
@@ -71809,9 +71784,6 @@
       </c>
     </row>
     <row r="53" spans="4:17">
-      <c r="D53" s="148" t="s">
-        <v>395</v>
-      </c>
       <c r="F53" s="146" t="s">
         <v>295</v>
       </c>
@@ -72708,7 +72680,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="XebqJ450Kj8JT3wXYN5dW/jEy3ZJbPUyRlEG1JszK4QeYgN9DfeWhyGHadfktHkuQ2RrK3ANNzdQR0Ox0xdzWw==" saltValue="A4cG2nJTrxp5K9O7XCKUdQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="uEojSY1baWnb9PvfGgyg3oyrouI7fbABX0u+mgpxmQS2efMviSbpz8Y5NZaVEgWoWH8LjI69hYgPt947Faav+A==" saltValue="fJBfq3VHmHs3ltIwtF6nOg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="45" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>